<commit_message>
fix many bugs;clean more data;describe the data
</commit_message>
<xml_diff>
--- a/btc_data.xlsx
+++ b/btc_data.xlsx
@@ -7615,9 +7615,6 @@
       <c r="I4">
         <v>0.04066198171888972</v>
       </c>
-      <c r="J4">
-        <v>0.07292131904674085</v>
-      </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1">
@@ -7647,9 +7644,6 @@
       <c r="I5">
         <v>0.04783732941416006</v>
       </c>
-      <c r="J5">
-        <v>0.06880823006445744</v>
-      </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1">
@@ -7679,9 +7673,6 @@
       <c r="I6">
         <v>0.005286004429237438</v>
       </c>
-      <c r="J6">
-        <v>0.06363910929918738</v>
-      </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1">
@@ -7711,9 +7702,6 @@
       <c r="I7">
         <v>-0.06902858641043601</v>
       </c>
-      <c r="J7">
-        <v>0.05512257682734612</v>
-      </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1">
@@ -7743,9 +7731,6 @@
       <c r="I8">
         <v>0.002796087302001188</v>
       </c>
-      <c r="J8">
-        <v>0.05750193863357553</v>
-      </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="1">
@@ -7775,9 +7760,6 @@
       <c r="I9">
         <v>-0.02010067170700291</v>
       </c>
-      <c r="J9">
-        <v>0.05266903509610542</v>
-      </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1">
@@ -7807,9 +7789,6 @@
       <c r="I10">
         <v>-0.006923915072824198</v>
       </c>
-      <c r="J10">
-        <v>0.04898177018104545</v>
-      </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="1">
@@ -7839,9 +7818,6 @@
       <c r="I11">
         <v>-0.01440323031074374</v>
       </c>
-      <c r="J11">
-        <v>0.04582178601530966</v>
-      </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="1">
@@ -7871,9 +7847,6 @@
       <c r="I12">
         <v>-0.07343127808588294</v>
       </c>
-      <c r="J12">
-        <v>0.04324230636964466</v>
-      </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="1">
@@ -7903,9 +7876,6 @@
       <c r="I13">
         <v>-0.1730447200137455</v>
       </c>
-      <c r="J13">
-        <v>0.04538570488857263</v>
-      </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="1">
@@ -7935,9 +7905,6 @@
       <c r="I14">
         <v>0.1327811112338184</v>
       </c>
-      <c r="J14">
-        <v>0.06290439047108085</v>
-      </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="1">
@@ -7967,9 +7934,6 @@
       <c r="I15">
         <v>-0.003405793134832821</v>
       </c>
-      <c r="J15">
-        <v>0.07494987611573825</v>
-      </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="1">
@@ -7999,9 +7963,6 @@
       <c r="I16">
         <v>-0.005213567052887434</v>
       </c>
-      <c r="J16">
-        <v>0.07208441263263352</v>
-      </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="1">
@@ -8031,9 +7992,6 @@
       <c r="I17">
         <v>0.1079571415050924</v>
       </c>
-      <c r="J17">
-        <v>0.06950654869427586</v>
-      </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="1">
@@ -8063,9 +8021,6 @@
       <c r="I18">
         <v>-0.04614865602598025</v>
       </c>
-      <c r="J18">
-        <v>0.07376597429449033</v>
-      </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="1">
@@ -8095,9 +8050,6 @@
       <c r="I19">
         <v>-0.006923915072824198</v>
       </c>
-      <c r="J19">
-        <v>0.07206654732397763</v>
-      </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="1">
@@ -8127,9 +8079,6 @@
       <c r="I20">
         <v>-0.07224816420762409</v>
       </c>
-      <c r="J20">
-        <v>0.06991633374676935</v>
-      </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="1">
@@ -8159,9 +8108,6 @@
       <c r="I21">
         <v>-0.0014009809156281</v>
       </c>
-      <c r="J21">
-        <v>0.06948970103423813</v>
-      </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="1">
@@ -8191,9 +8137,6 @@
       <c r="I22">
         <v>0.04907583764659264</v>
       </c>
-      <c r="J22">
-        <v>0.06767867099149992</v>
-      </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="1">
@@ -8223,9 +8166,6 @@
       <c r="I23">
         <v>-0.03407398033375144</v>
       </c>
-      <c r="J23">
-        <v>0.06727955186406197</v>
-      </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="1">
@@ -8255,9 +8195,6 @@
       <c r="I24">
         <v>0.0731575206177265</v>
       </c>
-      <c r="J24">
-        <v>0.06588086960488707</v>
-      </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="1">
@@ -8287,9 +8224,6 @@
       <c r="I25">
         <v>-0.01308523954865548</v>
       </c>
-      <c r="J25">
-        <v>0.06665207552985919</v>
-      </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="1">
@@ -8319,9 +8253,6 @@
       <c r="I26">
         <v>0.08075014968510907</v>
       </c>
-      <c r="J26">
-        <v>0.06520203151574046</v>
-      </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="1">
@@ -8351,9 +8282,6 @@
       <c r="I27">
         <v>-0.003706861931326512</v>
       </c>
-      <c r="J27">
-        <v>0.06617236913390706</v>
-      </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="1">
@@ -8383,9 +8311,6 @@
       <c r="I28">
         <v>-0.004811556997222082</v>
       </c>
-      <c r="J28">
-        <v>0.06483555354089915</v>
-      </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="1">
@@ -8415,9 +8340,6 @@
       <c r="I29">
         <v>0.04621542379696289</v>
       </c>
-      <c r="J29">
-        <v>0.06357739315235272</v>
-      </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="1">
@@ -8447,9 +8369,6 @@
       <c r="I30">
         <v>0.008464078412129364</v>
       </c>
-      <c r="J30">
-        <v>0.06308165041672005</v>
-      </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="1">
@@ -8480,7 +8399,7 @@
         <v>-0.001000500333583534</v>
       </c>
       <c r="J31">
-        <v>0.06197177993629523</v>
+        <v>0.06089392769641348</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -8512,7 +8431,7 @@
         <v>-0.02040680977766262</v>
       </c>
       <c r="J32">
-        <v>0.06089392769641347</v>
+        <v>0.06093153349688687</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -8544,7 +8463,7 @@
         <v>-0.02255240447051149</v>
       </c>
       <c r="J33">
-        <v>0.06093153349688687</v>
+        <v>0.05879413492188225</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -8576,7 +8495,7 @@
         <v>0.02352119504134587</v>
       </c>
       <c r="J34">
-        <v>0.05879413492188225</v>
+        <v>0.05846877306427052</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -8608,7 +8527,7 @@
         <v>0.01281750371061434</v>
       </c>
       <c r="J35">
-        <v>0.05846877306427053</v>
+        <v>0.05781703538617503</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -8640,7 +8559,7 @@
         <v>0.01479008547263535</v>
       </c>
       <c r="J36">
-        <v>0.05781703538617504</v>
+        <v>0.05788227488393095</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -8672,7 +8591,7 @@
         <v>0.03912455468405008</v>
       </c>
       <c r="J37">
-        <v>0.05788227488393095</v>
+        <v>0.05687908233798154</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -8704,7 +8623,7 @@
         <v>0.03604259134692931</v>
       </c>
       <c r="J38">
-        <v>0.05687908233798154</v>
+        <v>0.05721227827272047</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -8736,7 +8655,7 @@
         <v>-0.001100605444033004</v>
       </c>
       <c r="J39">
-        <v>0.05721227827272048</v>
+        <v>0.05704815679899874</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -8768,7 +8687,7 @@
         <v>0.009950330853168092</v>
       </c>
       <c r="J40">
-        <v>0.05704815679899873</v>
+        <v>0.05701963967702504</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -8800,7 +8719,7 @@
         <v>0.1178719205948891</v>
       </c>
       <c r="J41">
-        <v>0.05701963967702504</v>
+        <v>0.06050786826817987</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -8832,7 +8751,7 @@
         <v>0.03768106696768848</v>
       </c>
       <c r="J42">
-        <v>0.06050786826817986</v>
+        <v>0.05866070804829954</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -8864,7 +8783,7 @@
         <v>0.03459464476449896</v>
       </c>
       <c r="J43">
-        <v>0.05866070804829953</v>
+        <v>0.04709907257325442</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -8896,7 +8815,7 @@
         <v>-0.02367812735457715</v>
       </c>
       <c r="J44">
-        <v>0.04709907257325441</v>
+        <v>0.04258293138726081</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -8928,7 +8847,7 @@
         <v>0.01143437762566317</v>
       </c>
       <c r="J45">
-        <v>0.04258293138726081</v>
+        <v>0.0424548558612246</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -8960,7 +8879,7 @@
         <v>-0.02942881069081217</v>
       </c>
       <c r="J46">
-        <v>0.04245485586122459</v>
+        <v>0.04307616647254156</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -8992,7 +8911,7 @@
         <v>-0.005716306996109192</v>
       </c>
       <c r="J47">
-        <v>0.04307616647254155</v>
+        <v>0.03937574651534794</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -9024,7 +8943,7 @@
         <v>0.02293497128249599</v>
       </c>
       <c r="J48">
-        <v>0.03937574651534793</v>
+        <v>0.03795468268153515</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -9056,7 +8975,7 @@
         <v>0.04974209189481401</v>
       </c>
       <c r="J49">
-        <v>0.03795468268153515</v>
+        <v>0.03835694169848473</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -9088,7 +9007,7 @@
         <v>0.003394233068015617</v>
       </c>
       <c r="J50">
-        <v>0.03835694169848472</v>
+        <v>0.03477711022024747</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -9120,7 +9039,7 @@
         <v>-0.004108428044543191</v>
       </c>
       <c r="J51">
-        <v>0.03477711022024746</v>
+        <v>0.0348300346634959</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -9152,7 +9071,7 @@
         <v>-0.0123762710680554</v>
       </c>
       <c r="J52">
-        <v>0.03483003466349589</v>
+        <v>0.03468101097645844</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -9184,7 +9103,7 @@
         <v>-0.06967167324931926</v>
       </c>
       <c r="J53">
-        <v>0.03468101097645842</v>
+        <v>0.03694859124838352</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -9216,7 +9135,7 @@
         <v>0.0374884444109916</v>
       </c>
       <c r="J54">
-        <v>0.03694859124838352</v>
+        <v>0.03551525382049273</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -9248,7 +9167,7 @@
         <v>0.02926749768056814</v>
       </c>
       <c r="J55">
-        <v>0.03551525382049271</v>
+        <v>0.03530406129083265</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -9280,7 +9199,7 @@
         <v>-0.02234786366390762</v>
       </c>
       <c r="J56">
-        <v>0.03530406129083264</v>
+        <v>0.03354832069904402</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -9312,7 +9231,7 @@
         <v>-0.006823225348125537</v>
       </c>
       <c r="J57">
-        <v>0.03354832069904401</v>
+        <v>0.0335985537679715</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -9344,7 +9263,7 @@
         <v>0.07334339422420959</v>
       </c>
       <c r="J58">
-        <v>0.03359855376797149</v>
+        <v>0.03536386085538738</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -9376,7 +9295,7 @@
         <v>-0.005012541823544286</v>
       </c>
       <c r="J59">
-        <v>0.03536386085538738</v>
+        <v>0.03493805772399827</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -9408,7 +9327,7 @@
         <v>0.05297188476610572</v>
       </c>
       <c r="J60">
-        <v>0.03493805772399827</v>
+        <v>0.03575013734450242</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -9440,7 +9359,7 @@
         <v>0.04085399400826612</v>
       </c>
       <c r="J61">
-        <v>0.03575013734450241</v>
+        <v>0.03601042588304022</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -9472,7 +9391,7 @@
         <v>0.04258044753511848</v>
       </c>
       <c r="J62">
-        <v>0.03601042588304022</v>
+        <v>0.03576128519281951</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -9504,7 +9423,7 @@
         <v>0.03613904661587314</v>
       </c>
       <c r="J63">
-        <v>0.0357612851928195</v>
+        <v>0.03516561438476325</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -9536,7 +9455,7 @@
         <v>0.0123237496888319</v>
       </c>
       <c r="J64">
-        <v>0.03516561438476324</v>
+        <v>0.03516671512426051</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -9568,7 +9487,7 @@
         <v>0.001798381941379397</v>
       </c>
       <c r="J65">
-        <v>0.0351667151242605</v>
+        <v>0.03527830848310094</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -9600,7 +9519,7 @@
         <v>-0.05953771271619628</v>
       </c>
       <c r="J66">
-        <v>0.03527830848310094</v>
+        <v>0.03797952495345832</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -9632,7 +9551,7 @@
         <v>0.02107632560191631</v>
       </c>
       <c r="J67">
-        <v>0.03797952495345831</v>
+        <v>0.03772616270328276</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -9664,7 +9583,7 @@
         <v>0.04659728537678226</v>
       </c>
       <c r="J68">
-        <v>0.03772616270328276</v>
+        <v>0.03798339333833314</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -9696,7 +9615,7 @@
         <v>-0.04342955792733598</v>
       </c>
       <c r="J69">
-        <v>0.03798339333833313</v>
+        <v>0.03935364633920976</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -9728,7 +9647,7 @@
         <v>-0.08555788836164654</v>
       </c>
       <c r="J70">
-        <v>0.03935364633920976</v>
+        <v>0.04330166555898175</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -9760,7 +9679,7 @@
         <v>-0.03759803041531849</v>
       </c>
       <c r="J71">
-        <v>0.04330166555898175</v>
+        <v>0.03906015578766227</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -9792,7 +9711,7 @@
         <v>-0.07904320734045285</v>
       </c>
       <c r="J72">
-        <v>0.03906015578766227</v>
+        <v>0.04143043596792111</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -9824,7 +9743,7 @@
         <v>0.1062501198426593</v>
       </c>
       <c r="J73">
-        <v>0.04143043596792111</v>
+        <v>0.04531317248799566</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -9856,7 +9775,7 @@
         <v>0.01607018017749446</v>
       </c>
       <c r="J74">
-        <v>0.04531317248799566</v>
+        <v>0.04507270845080218</v>
       </c>
     </row>
     <row r="75" spans="1:10">
@@ -9888,7 +9807,7 @@
         <v>0.1010211140587282</v>
       </c>
       <c r="J75">
-        <v>0.04507270845080218</v>
+        <v>0.0483750377421812</v>
       </c>
     </row>
     <row r="76" spans="1:10">
@@ -9920,7 +9839,7 @@
         <v>0.07742389696480363</v>
       </c>
       <c r="J76">
-        <v>0.0483750377421812</v>
+        <v>0.04946290509351739</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -9952,7 +9871,7 @@
         <v>-0.02398536275051131</v>
       </c>
       <c r="J77">
-        <v>0.04946290509351739</v>
+        <v>0.04979144484184603</v>
       </c>
     </row>
     <row r="78" spans="1:10">
@@ -9984,7 +9903,7 @@
         <v>0.0123237496888319</v>
       </c>
       <c r="J78">
-        <v>0.04979144484184602</v>
+        <v>0.04973938830070692</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -10016,7 +9935,7 @@
         <v>0.03546366427556906</v>
       </c>
       <c r="J79">
-        <v>0.04973938830070692</v>
+        <v>0.04941694557964673</v>
       </c>
     </row>
     <row r="80" spans="1:10">
@@ -10048,7 +9967,7 @@
         <v>0.02342351494358811</v>
       </c>
       <c r="J80">
-        <v>0.04941694557964674</v>
+        <v>0.04946134965865834</v>
       </c>
     </row>
     <row r="81" spans="1:10">
@@ -10080,7 +9999,7 @@
         <v>-0.01806214281840852</v>
       </c>
       <c r="J81">
-        <v>0.04946134965865833</v>
+        <v>0.04966925729249039</v>
       </c>
     </row>
     <row r="82" spans="1:10">
@@ -10112,7 +10031,7 @@
         <v>0.01626697246387194</v>
       </c>
       <c r="J82">
-        <v>0.04966925729249039</v>
+        <v>0.04949732643037694</v>
       </c>
     </row>
     <row r="83" spans="1:10">
@@ -10144,7 +10063,7 @@
         <v>-0.03118111748357474</v>
       </c>
       <c r="J83">
-        <v>0.04949732643037693</v>
+        <v>0.04780253035484624</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -10176,7 +10095,7 @@
         <v>0.02654455522211221</v>
       </c>
       <c r="J84">
-        <v>0.04780253035484624</v>
+        <v>0.04764547193541456</v>
       </c>
     </row>
     <row r="85" spans="1:10">
@@ -10208,7 +10127,7 @@
         <v>0.06775210205081852</v>
       </c>
       <c r="J85">
-        <v>0.04764547193541455</v>
+        <v>0.04863500680353701</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -10240,7 +10159,7 @@
         <v>0.0608128393965124</v>
       </c>
       <c r="J86">
-        <v>0.048635006803537</v>
+        <v>0.04890498781612944</v>
       </c>
     </row>
     <row r="87" spans="1:10">
@@ -10272,7 +10191,7 @@
         <v>0.04334680450336587</v>
       </c>
       <c r="J87">
-        <v>0.04890498781612944</v>
+        <v>0.04895444291636381</v>
       </c>
     </row>
     <row r="88" spans="1:10">
@@ -10304,7 +10223,7 @@
         <v>0.01725035340652767</v>
       </c>
       <c r="J88">
-        <v>0.04895444291636381</v>
+        <v>0.04781380294902777</v>
       </c>
     </row>
     <row r="89" spans="1:10">
@@ -10336,7 +10255,7 @@
         <v>-0.01511363781004818</v>
       </c>
       <c r="J89">
-        <v>0.04781380294902776</v>
+        <v>0.0480008325202385</v>
       </c>
     </row>
     <row r="90" spans="1:10">
@@ -10368,7 +10287,7 @@
         <v>0.01607018017749446</v>
       </c>
       <c r="J90">
-        <v>0.04800083252023849</v>
+        <v>0.04747724464563424</v>
       </c>
     </row>
     <row r="91" spans="1:10">
@@ -10400,7 +10319,7 @@
         <v>0.09267033484130814</v>
       </c>
       <c r="J91">
-        <v>0.04747724464563423</v>
+        <v>0.04938230097517576</v>
       </c>
     </row>
     <row r="92" spans="1:10">
@@ -10432,7 +10351,7 @@
         <v>0.001099395443301064</v>
       </c>
       <c r="J92">
-        <v>0.04938230097517574</v>
+        <v>0.0491924621769986</v>
       </c>
     </row>
     <row r="93" spans="1:10">
@@ -10464,7 +10383,7 @@
         <v>0.02508278036746324</v>
       </c>
       <c r="J93">
-        <v>0.0491924621769986</v>
+        <v>0.04906684192333723</v>
       </c>
     </row>
     <row r="94" spans="1:10">
@@ -10496,7 +10415,7 @@
         <v>0.03854740961223883</v>
       </c>
       <c r="J94">
-        <v>0.04906684192333721</v>
+        <v>0.04926473885412468</v>
       </c>
     </row>
     <row r="95" spans="1:10">
@@ -10528,7 +10447,7 @@
         <v>0</v>
       </c>
       <c r="J95">
-        <v>0.04926473885412465</v>
+        <v>0.04928258958246998</v>
       </c>
     </row>
     <row r="96" spans="1:10">
@@ -10560,7 +10479,7 @@
         <v>0.1540935353374003</v>
       </c>
       <c r="J96">
-        <v>0.04928258958246997</v>
+        <v>0.05339563679053817</v>
       </c>
     </row>
     <row r="97" spans="1:10">
@@ -10592,7 +10511,7 @@
         <v>0.2047351516308547</v>
       </c>
       <c r="J97">
-        <v>0.05339563679053815</v>
+        <v>0.06294080162804776</v>
       </c>
     </row>
     <row r="98" spans="1:10">
@@ -10624,7 +10543,7 @@
         <v>-0.04510197391242018</v>
       </c>
       <c r="J98">
-        <v>0.06294080162804773</v>
+        <v>0.06423469733315235</v>
       </c>
     </row>
     <row r="99" spans="1:10">
@@ -10656,7 +10575,7 @@
         <v>-0.07925968098563209</v>
       </c>
       <c r="J99">
-        <v>0.06423469733315233</v>
+        <v>0.06586784517869597</v>
       </c>
     </row>
     <row r="100" spans="1:10">
@@ -10688,7 +10607,7 @@
         <v>0.02273948696948934</v>
       </c>
       <c r="J100">
-        <v>0.06586784517869596</v>
+        <v>0.06253733138329565</v>
       </c>
     </row>
     <row r="101" spans="1:10">
@@ -10720,7 +10639,7 @@
         <v>0.1108255550888846</v>
       </c>
       <c r="J101">
-        <v>0.06253733138329563</v>
+        <v>0.06306585245449259</v>
       </c>
     </row>
     <row r="102" spans="1:10">
@@ -10752,7 +10671,7 @@
         <v>0.0126200313561022</v>
       </c>
       <c r="J102">
-        <v>0.06306585245449257</v>
+        <v>0.05959526293487016</v>
       </c>
     </row>
     <row r="103" spans="1:10">
@@ -10784,7 +10703,7 @@
         <v>-0.04740612239727035</v>
       </c>
       <c r="J103">
-        <v>0.05959526293487015</v>
+        <v>0.05992108437312035</v>
       </c>
     </row>
     <row r="104" spans="1:10">
@@ -10816,7 +10735,7 @@
         <v>0.01242251999855711</v>
       </c>
       <c r="J104">
-        <v>0.05992108437312033</v>
+        <v>0.05995514051696439</v>
       </c>
     </row>
     <row r="105" spans="1:10">
@@ -10848,7 +10767,7 @@
         <v>0.06719124954032338</v>
       </c>
       <c r="J105">
-        <v>0.05995514051696437</v>
+        <v>0.0588900241994918</v>
       </c>
     </row>
     <row r="106" spans="1:10">
@@ -10880,7 +10799,7 @@
         <v>0.09075436326846412</v>
       </c>
       <c r="J106">
-        <v>0.05889002419949178</v>
+        <v>0.05931452647510221</v>
       </c>
     </row>
     <row r="107" spans="1:10">
@@ -10912,7 +10831,7 @@
         <v>-0.01136433007904976</v>
       </c>
       <c r="J107">
-        <v>0.05931452647510218</v>
+        <v>0.05896411832873551</v>
       </c>
     </row>
     <row r="108" spans="1:10">
@@ -10944,7 +10863,7 @@
         <v>-0.002002002670673079</v>
       </c>
       <c r="J108">
-        <v>0.05896411832873549</v>
+        <v>0.05917112262687682</v>
       </c>
     </row>
     <row r="109" spans="1:10">
@@ -10976,7 +10895,7 @@
         <v>-0.08762974996097406</v>
       </c>
       <c r="J109">
-        <v>0.05917112262687681</v>
+        <v>0.06290579404077022</v>
       </c>
     </row>
     <row r="110" spans="1:10">
@@ -11008,7 +10927,7 @@
         <v>-0.05445618579605885</v>
       </c>
       <c r="J110">
-        <v>0.06290579404077021</v>
+        <v>0.06458210070622378</v>
       </c>
     </row>
     <row r="111" spans="1:10">
@@ -11040,7 +10959,7 @@
         <v>-0.0473012731180131</v>
       </c>
       <c r="J111">
-        <v>0.06458210070622376</v>
+        <v>0.06543772811178246</v>
       </c>
     </row>
     <row r="112" spans="1:10">
@@ -11072,7 +10991,7 @@
         <v>-0.1736393564111207</v>
       </c>
       <c r="J112">
-        <v>0.06543772811178244</v>
+        <v>0.07456093445610945</v>
       </c>
     </row>
     <row r="113" spans="1:10">
@@ -11104,7 +11023,7 @@
         <v>0.06363186024477352</v>
       </c>
       <c r="J113">
-        <v>0.07456093445610944</v>
+        <v>0.07451597790429586</v>
       </c>
     </row>
     <row r="114" spans="1:10">
@@ -11136,7 +11055,7 @@
         <v>-0.04061368288529713</v>
       </c>
       <c r="J114">
-        <v>0.07451597790429584</v>
+        <v>0.07528109772041473</v>
       </c>
     </row>
     <row r="115" spans="1:10">
@@ -11168,7 +11087,7 @@
         <v>0.01084102317787477</v>
       </c>
       <c r="J115">
-        <v>0.07528109772041472</v>
+        <v>0.07466195405695933</v>
       </c>
     </row>
     <row r="116" spans="1:10">
@@ -11200,7 +11119,7 @@
         <v>0.1405442449923084</v>
       </c>
       <c r="J116">
-        <v>0.07466195405695933</v>
+        <v>0.0777167946251467</v>
       </c>
     </row>
     <row r="117" spans="1:10">
@@ -11232,7 +11151,7 @@
         <v>-0.01969263334573605</v>
       </c>
       <c r="J117">
-        <v>0.07771679462514669</v>
+        <v>0.07784185803009115</v>
       </c>
     </row>
     <row r="118" spans="1:10">
@@ -11264,7 +11183,7 @@
         <v>-0.0713885960876529</v>
       </c>
       <c r="J118">
-        <v>0.07784185803009115</v>
+        <v>0.07942940261861642</v>
       </c>
     </row>
     <row r="119" spans="1:10">
@@ -11296,7 +11215,7 @@
         <v>9.999500033329732e-05</v>
       </c>
       <c r="J119">
-        <v>0.07942940261861639</v>
+        <v>0.07929682103667778</v>
       </c>
     </row>
     <row r="120" spans="1:10">
@@ -11328,7 +11247,7 @@
         <v>-0.1456039738587918</v>
       </c>
       <c r="J120">
-        <v>0.07929682103667776</v>
+        <v>0.08439697924679482</v>
       </c>
     </row>
     <row r="121" spans="1:10">
@@ -11360,7 +11279,7 @@
         <v>0.1088544049120821</v>
       </c>
       <c r="J121">
-        <v>0.0843969792467948</v>
+        <v>0.08501022544635013</v>
       </c>
     </row>
     <row r="122" spans="1:10">
@@ -11392,7 +11311,7 @@
         <v>-0.03283315709524021</v>
       </c>
       <c r="J122">
-        <v>0.0850102254463501</v>
+        <v>0.08532971513248004</v>
       </c>
     </row>
     <row r="123" spans="1:10">
@@ -11424,7 +11343,7 @@
         <v>0.09667288726026069</v>
       </c>
       <c r="J123">
-        <v>0.08532971513248004</v>
+        <v>0.08684556021442132</v>
       </c>
     </row>
     <row r="124" spans="1:10">
@@ -11456,7 +11375,7 @@
         <v>0.02985002196888529</v>
       </c>
       <c r="J124">
-        <v>0.08684556021442132</v>
+        <v>0.08675871871957104</v>
       </c>
     </row>
     <row r="125" spans="1:10">
@@ -11488,7 +11407,7 @@
         <v>0.0002999550089979424</v>
       </c>
       <c r="J125">
-        <v>0.08675871871957104</v>
+        <v>0.08675767263023632</v>
       </c>
     </row>
     <row r="126" spans="1:10">
@@ -11520,7 +11439,7 @@
         <v>0.1096612542095184</v>
       </c>
       <c r="J126">
-        <v>0.0867576726302363</v>
+        <v>0.08454511066140806</v>
       </c>
     </row>
     <row r="127" spans="1:10">
@@ -11552,7 +11471,7 @@
         <v>0.01429730470082439</v>
       </c>
       <c r="J127">
-        <v>0.08454511066140806</v>
+        <v>0.07593199013340615</v>
       </c>
     </row>
     <row r="128" spans="1:10">
@@ -11584,7 +11503,7 @@
         <v>-0.05784099968984994</v>
       </c>
       <c r="J128">
-        <v>0.07593199013340614</v>
+        <v>0.07623429576696732</v>
       </c>
     </row>
     <row r="129" spans="1:10">
@@ -11616,7 +11535,7 @@
         <v>-0.0814269986957292</v>
       </c>
       <c r="J129">
-        <v>0.07623429576696732</v>
+        <v>0.07631364491336444</v>
       </c>
     </row>
     <row r="130" spans="1:10">
@@ -11648,7 +11567,7 @@
         <v>-0.03459144476961909</v>
       </c>
       <c r="J130">
-        <v>0.07631364491336441</v>
+        <v>0.07645790562303201</v>
       </c>
     </row>
     <row r="131" spans="1:10">
@@ -11680,7 +11599,7 @@
         <v>0.03227356055029564</v>
       </c>
       <c r="J131">
-        <v>0.07645790562303201</v>
+        <v>0.07378363517895405</v>
       </c>
     </row>
     <row r="132" spans="1:10">
@@ -11712,7 +11631,7 @@
         <v>-0.115859886094535</v>
       </c>
       <c r="J132">
-        <v>0.07378363517895403</v>
+        <v>0.07646994967472419</v>
       </c>
     </row>
     <row r="133" spans="1:10">
@@ -11744,7 +11663,7 @@
         <v>0.03825871211709027</v>
       </c>
       <c r="J133">
-        <v>0.07646994967472419</v>
+        <v>0.07655515926775552</v>
       </c>
     </row>
     <row r="134" spans="1:10">
@@ -11776,7 +11695,7 @@
         <v>0.02917037729977992</v>
       </c>
       <c r="J134">
-        <v>0.07655515926775552</v>
+        <v>0.07675007035895992</v>
       </c>
     </row>
     <row r="135" spans="1:10">
@@ -11808,7 +11727,7 @@
         <v>-0.04562517802627555</v>
       </c>
       <c r="J135">
-        <v>0.07675007035895991</v>
+        <v>0.07586001393167695</v>
       </c>
     </row>
     <row r="136" spans="1:10">
@@ -11840,7 +11759,7 @@
         <v>0.001299155731620129</v>
       </c>
       <c r="J136">
-        <v>0.07586001393167693</v>
+        <v>0.07354460686122756</v>
       </c>
     </row>
     <row r="137" spans="1:10">
@@ -11872,7 +11791,7 @@
         <v>-0.2038312402818369</v>
       </c>
       <c r="J137">
-        <v>0.07354460686122755</v>
+        <v>0.08149416477311437</v>
       </c>
     </row>
     <row r="138" spans="1:10">
@@ -11904,7 +11823,7 @@
         <v>0.0008995952428359939</v>
       </c>
       <c r="J138">
-        <v>0.08149416477311437</v>
+        <v>0.08151546746278548</v>
       </c>
     </row>
     <row r="139" spans="1:10">
@@ -11936,7 +11855,7 @@
         <v>-0.003305457008726481</v>
       </c>
       <c r="J139">
-        <v>0.0815154674627855</v>
+        <v>0.08047374689216731</v>
       </c>
     </row>
     <row r="140" spans="1:10">
@@ -11968,7 +11887,7 @@
         <v>0.03825871211709027</v>
       </c>
       <c r="J140">
-        <v>0.0804737468921673</v>
+        <v>0.08068804094789593</v>
       </c>
     </row>
     <row r="141" spans="1:10">
@@ -12000,7 +11919,7 @@
         <v>0.1035488756285588</v>
       </c>
       <c r="J141">
-        <v>0.08068804094789594</v>
+        <v>0.08307441759393379</v>
       </c>
     </row>
     <row r="142" spans="1:10">
@@ -12032,7 +11951,7 @@
         <v>-0.1002624219383942</v>
       </c>
       <c r="J142">
-        <v>0.08307441759393379</v>
+        <v>0.07897584332451894</v>
       </c>
     </row>
     <row r="143" spans="1:10">
@@ -12064,7 +11983,7 @@
         <v>-0.06667413326799275</v>
       </c>
       <c r="J143">
-        <v>0.07897584332451894</v>
+        <v>0.07868336985807452</v>
       </c>
     </row>
     <row r="144" spans="1:10">
@@ -12096,7 +12015,7 @@
         <v>0.004489905272852001</v>
       </c>
       <c r="J144">
-        <v>0.07868336985807452</v>
+        <v>0.07848566138659199</v>
       </c>
     </row>
     <row r="145" spans="1:10">
@@ -12128,7 +12047,7 @@
         <v>0.05354076692802976</v>
       </c>
       <c r="J145">
-        <v>0.07848566138659199</v>
+        <v>0.07921020762554117</v>
       </c>
     </row>
     <row r="146" spans="1:10">
@@ -12160,7 +12079,7 @@
         <v>-0.02378052866540339</v>
       </c>
       <c r="J146">
-        <v>0.07921020762554117</v>
+        <v>0.07426143878203455</v>
       </c>
     </row>
     <row r="147" spans="1:10">
@@ -12192,7 +12111,7 @@
         <v>-0.006823225348125537</v>
       </c>
       <c r="J147">
-        <v>0.07426143878203455</v>
+        <v>0.07424890217117221</v>
       </c>
     </row>
     <row r="148" spans="1:10">
@@ -12224,7 +12143,7 @@
         <v>0.03469123978993026</v>
       </c>
       <c r="J148">
-        <v>0.07424890217117219</v>
+        <v>0.07379570563955259</v>
       </c>
     </row>
     <row r="149" spans="1:10">
@@ -12256,7 +12175,7 @@
         <v>0.03246719013750141</v>
       </c>
       <c r="J149">
-        <v>0.07379570563955257</v>
+        <v>0.07414506531638675</v>
       </c>
     </row>
     <row r="150" spans="1:10">
@@ -12288,7 +12207,7 @@
         <v>-0.05445618579605885</v>
       </c>
       <c r="J150">
-        <v>0.07414506531638675</v>
+        <v>0.06999244791333403</v>
       </c>
     </row>
     <row r="151" spans="1:10">
@@ -12320,7 +12239,7 @@
         <v>-0.09706171284313124</v>
       </c>
       <c r="J151">
-        <v>0.069992447913334</v>
+        <v>0.06870016538435601</v>
       </c>
     </row>
     <row r="152" spans="1:10">
@@ -12352,7 +12271,7 @@
         <v>0.01064316009847976</v>
       </c>
       <c r="J152">
-        <v>0.06870016538435601</v>
+        <v>0.06866386192522952</v>
       </c>
     </row>
     <row r="153" spans="1:10">
@@ -12384,7 +12303,7 @@
         <v>-0.1133926873550905</v>
       </c>
       <c r="J153">
-        <v>0.06866386192522951</v>
+        <v>0.06825666875178958</v>
       </c>
     </row>
     <row r="154" spans="1:10">
@@ -12416,7 +12335,7 @@
         <v>-0.03159387159117863</v>
       </c>
       <c r="J154">
-        <v>0.06825666875178957</v>
+        <v>0.06776252173397558</v>
       </c>
     </row>
     <row r="155" spans="1:10">
@@ -12448,7 +12367,7 @@
         <v>0.03575316970581784</v>
       </c>
       <c r="J155">
-        <v>0.06776252173397557</v>
+        <v>0.06839450634882248</v>
       </c>
     </row>
     <row r="156" spans="1:10">
@@ -12480,7 +12399,7 @@
         <v>-0.117208200905541</v>
       </c>
       <c r="J156">
-        <v>0.06839450634882248</v>
+        <v>0.06647060269194253</v>
       </c>
     </row>
     <row r="157" spans="1:10">
@@ -12512,7 +12431,7 @@
         <v>-0.1654644397275317</v>
       </c>
       <c r="J157">
-        <v>0.06647060269194251</v>
+        <v>0.07084480547315382</v>
       </c>
     </row>
     <row r="158" spans="1:10">
@@ -12544,7 +12463,7 @@
         <v>0.09912109086780725</v>
       </c>
       <c r="J158">
-        <v>0.0708448054731538</v>
+        <v>0.07443288105065916</v>
       </c>
     </row>
     <row r="159" spans="1:10">
@@ -12576,7 +12495,7 @@
         <v>-0.01136433007904976</v>
       </c>
       <c r="J159">
-        <v>0.07443288105065915</v>
+        <v>0.07369353503820379</v>
       </c>
     </row>
     <row r="160" spans="1:10">
@@ -12608,7 +12527,7 @@
         <v>0.08194858264716733</v>
       </c>
       <c r="J160">
-        <v>0.07369353503820378</v>
+        <v>0.07607087487862481</v>
       </c>
     </row>
     <row r="161" spans="1:10">
@@ -12640,7 +12559,7 @@
         <v>0.05297188476610572</v>
       </c>
       <c r="J161">
-        <v>0.07607087487862481</v>
+        <v>0.07664065840343288</v>
       </c>
     </row>
     <row r="162" spans="1:10">
@@ -12672,7 +12591,7 @@
         <v>-0.01389610519211135</v>
       </c>
       <c r="J162">
-        <v>0.07664065840343287</v>
+        <v>0.07437816146899175</v>
       </c>
     </row>
     <row r="163" spans="1:10">
@@ -12704,7 +12623,7 @@
         <v>-0.05943158376942647</v>
       </c>
       <c r="J163">
-        <v>0.07437816146899173</v>
+        <v>0.07412269236367879</v>
       </c>
     </row>
     <row r="164" spans="1:10">
@@ -12736,7 +12655,7 @@
         <v>0.09812439799319893</v>
       </c>
       <c r="J164">
-        <v>0.07412269236367877</v>
+        <v>0.07665666402914342</v>
       </c>
     </row>
     <row r="165" spans="1:10">
@@ -12768,7 +12687,7 @@
         <v>-0.04416089578576978</v>
       </c>
       <c r="J165">
-        <v>0.07665666402914342</v>
+        <v>0.07663731583628307</v>
       </c>
     </row>
     <row r="166" spans="1:10">
@@ -12800,7 +12719,7 @@
         <v>0.104630249078083</v>
       </c>
       <c r="J166">
-        <v>0.07663731583628305</v>
+        <v>0.07967993570928408</v>
       </c>
     </row>
     <row r="167" spans="1:10">
@@ -12832,7 +12751,7 @@
         <v>0.0557184887563437</v>
       </c>
       <c r="J167">
-        <v>0.07967993570928407</v>
+        <v>0.07184439753872279</v>
       </c>
     </row>
     <row r="168" spans="1:10">
@@ -12864,7 +12783,7 @@
         <v>0.01636535408626423</v>
       </c>
       <c r="J168">
-        <v>0.07184439753872279</v>
+        <v>0.07193176522008864</v>
       </c>
     </row>
     <row r="169" spans="1:10">
@@ -12896,7 +12815,7 @@
         <v>0.08406537511766743</v>
       </c>
       <c r="J169">
-        <v>0.07193176522008862</v>
+        <v>0.07366214326249662</v>
       </c>
     </row>
     <row r="170" spans="1:10">
@@ -12928,7 +12847,7 @@
         <v>-0.06368555168613305</v>
       </c>
       <c r="J170">
-        <v>0.07366214326249661</v>
+        <v>0.074187123350769</v>
       </c>
     </row>
     <row r="171" spans="1:10">
@@ -12960,7 +12879,7 @@
         <v>0.07436508195530674</v>
       </c>
       <c r="J171">
-        <v>0.074187123350769</v>
+        <v>0.07291721993419749</v>
       </c>
     </row>
     <row r="172" spans="1:10">
@@ -12992,7 +12911,7 @@
         <v>0.003992021269537457</v>
       </c>
       <c r="J172">
-        <v>0.07291721993419749</v>
+        <v>0.07063696195916078</v>
       </c>
     </row>
     <row r="173" spans="1:10">
@@ -13024,7 +12943,7 @@
         <v>-0.07042246429654593</v>
       </c>
       <c r="J173">
-        <v>0.07063696195916076</v>
+        <v>0.07076057812445942</v>
       </c>
     </row>
     <row r="174" spans="1:10">
@@ -13056,7 +12975,7 @@
         <v>-0.06166266039210687</v>
       </c>
       <c r="J174">
-        <v>0.07076057812445942</v>
+        <v>0.07160940869084215</v>
       </c>
     </row>
     <row r="175" spans="1:10">
@@ -13088,7 +13007,7 @@
         <v>0.03149866705937102</v>
       </c>
       <c r="J175">
-        <v>0.07160940869084215</v>
+        <v>0.07111854923500356</v>
       </c>
     </row>
     <row r="176" spans="1:10">
@@ -13120,7 +13039,7 @@
         <v>-0.04835026094104673</v>
       </c>
       <c r="J176">
-        <v>0.07111854923500356</v>
+        <v>0.07149544084611291</v>
       </c>
     </row>
     <row r="177" spans="1:10">
@@ -13152,7 +13071,7 @@
         <v>-0.01136433007904976</v>
       </c>
       <c r="J177">
-        <v>0.07149544084611291</v>
+        <v>0.07150477961170859</v>
       </c>
     </row>
     <row r="178" spans="1:10">
@@ -13184,7 +13103,7 @@
         <v>0.07686844425657707</v>
       </c>
       <c r="J178">
-        <v>0.07150477961170858</v>
+        <v>0.0727145658934731</v>
       </c>
     </row>
     <row r="179" spans="1:10">
@@ -13216,7 +13135,7 @@
         <v>0.02371652661731606</v>
       </c>
       <c r="J179">
-        <v>0.0727145658934731</v>
+        <v>0.07258274545903991</v>
       </c>
     </row>
     <row r="180" spans="1:10">
@@ -13248,7 +13167,7 @@
         <v>-0.02429269256904459</v>
       </c>
       <c r="J180">
-        <v>0.07258274545903989</v>
+        <v>0.07206377187398583</v>
       </c>
     </row>
     <row r="181" spans="1:10">
@@ -13280,7 +13199,7 @@
         <v>0.05741949086748642</v>
       </c>
       <c r="J181">
-        <v>0.07206377187398583</v>
+        <v>0.07059931344387871</v>
       </c>
     </row>
     <row r="182" spans="1:10">
@@ -13312,7 +13231,7 @@
         <v>0.009157937784765724</v>
       </c>
       <c r="J182">
-        <v>0.07059931344387869</v>
+        <v>0.07059382787123349</v>
       </c>
     </row>
     <row r="183" spans="1:10">
@@ -13344,7 +13263,7 @@
         <v>0.03691035402009715</v>
       </c>
       <c r="J183">
-        <v>0.07059382787123347</v>
+        <v>0.06735826426783187</v>
       </c>
     </row>
     <row r="184" spans="1:10">
@@ -13376,7 +13295,7 @@
         <v>0.005286004429237438</v>
       </c>
       <c r="J184">
-        <v>0.06735826426783187</v>
+        <v>0.06695884697437306</v>
       </c>
     </row>
     <row r="185" spans="1:10">
@@ -13408,7 +13327,7 @@
         <v>-0.007427515828796584</v>
       </c>
       <c r="J185">
-        <v>0.06695884697437304</v>
+        <v>0.06681796169907665</v>
       </c>
     </row>
     <row r="186" spans="1:10">
@@ -13440,7 +13359,7 @@
         <v>-0.06293979977387408</v>
       </c>
       <c r="J186">
-        <v>0.06681796169907665</v>
+        <v>0.06401182123304611</v>
       </c>
     </row>
     <row r="187" spans="1:10">
@@ -13472,7 +13391,7 @@
         <v>-0.07925968098563209</v>
       </c>
       <c r="J187">
-        <v>0.06401182123304611</v>
+        <v>0.05751921412207274</v>
       </c>
     </row>
     <row r="188" spans="1:10">
@@ -13504,7 +13423,7 @@
         <v>-0.06283330917156911</v>
       </c>
       <c r="J188">
-        <v>0.05751921412207273</v>
+        <v>0.05663407433722369</v>
       </c>
     </row>
     <row r="189" spans="1:10">
@@ -13536,7 +13455,7 @@
         <v>-0.008939841569474296</v>
       </c>
       <c r="J189">
-        <v>0.05663407433722367</v>
+        <v>0.05660957782360903</v>
       </c>
     </row>
     <row r="190" spans="1:10">
@@ -13568,7 +13487,7 @@
         <v>-0.05066191480222799</v>
       </c>
       <c r="J190">
-        <v>0.05660957782360902</v>
+        <v>0.05568320038566982</v>
       </c>
     </row>
     <row r="191" spans="1:10">
@@ -13600,7 +13519,7 @@
         <v>0.08378952572968316</v>
       </c>
       <c r="J191">
-        <v>0.05568320038566982</v>
+        <v>0.0569252570743534</v>
       </c>
     </row>
     <row r="192" spans="1:10">
@@ -13632,7 +13551,7 @@
         <v>-0.04363845702982949</v>
       </c>
       <c r="J192">
-        <v>0.05692525707435338</v>
+        <v>0.05748743688967139</v>
       </c>
     </row>
     <row r="193" spans="1:10">
@@ -13664,7 +13583,7 @@
         <v>0.001498876123735949</v>
       </c>
       <c r="J193">
-        <v>0.05748743688967138</v>
+        <v>0.05630290423296246</v>
       </c>
     </row>
     <row r="194" spans="1:10">
@@ -13696,7 +13615,7 @@
         <v>-0.1095916766300944</v>
       </c>
       <c r="J194">
-        <v>0.05630290423296245</v>
+        <v>0.05711094217173864</v>
       </c>
     </row>
     <row r="195" spans="1:10">
@@ -13728,7 +13647,7 @@
         <v>0.008067371077758793</v>
       </c>
       <c r="J195">
-        <v>0.05711094217173862</v>
+        <v>0.05660035415866584</v>
       </c>
     </row>
     <row r="196" spans="1:10">
@@ -13760,7 +13679,7 @@
         <v>-0.0002000200026670447</v>
       </c>
       <c r="J196">
-        <v>0.05660035415866584</v>
+        <v>0.05297004911487405</v>
       </c>
     </row>
     <row r="197" spans="1:10">
@@ -13792,7 +13711,7 @@
         <v>-0.04971559224593286</v>
       </c>
       <c r="J197">
-        <v>0.05297004911487403</v>
+        <v>0.05232711964819055</v>
       </c>
     </row>
     <row r="198" spans="1:10">
@@ -13824,7 +13743,7 @@
         <v>0.04353830201448341</v>
       </c>
       <c r="J198">
-        <v>0.05232711964819054</v>
+        <v>0.05299551226040389</v>
       </c>
     </row>
     <row r="199" spans="1:10">
@@ -13856,7 +13775,7 @@
         <v>0.04764665346735299</v>
       </c>
       <c r="J199">
-        <v>0.05299551226040389</v>
+        <v>0.05122117896787225</v>
       </c>
     </row>
     <row r="200" spans="1:10">
@@ -13888,7 +13807,7 @@
         <v>0.03420817132973696</v>
       </c>
       <c r="J200">
-        <v>0.05122117896787225</v>
+        <v>0.05069148363106112</v>
       </c>
     </row>
     <row r="201" spans="1:10">
@@ -13920,7 +13839,7 @@
         <v>0</v>
       </c>
       <c r="J201">
-        <v>0.0506914836310611</v>
+        <v>0.04843925135582691</v>
       </c>
     </row>
     <row r="202" spans="1:10">
@@ -13952,7 +13871,7 @@
         <v>-0.02204113087688028</v>
       </c>
       <c r="J202">
-        <v>0.04843925135582691</v>
+        <v>0.04845779143528563</v>
       </c>
     </row>
     <row r="203" spans="1:10">
@@ -13984,7 +13903,7 @@
         <v>0.02293497128249599</v>
       </c>
       <c r="J203">
-        <v>0.04845779143528563</v>
+        <v>0.04732570251743053</v>
       </c>
     </row>
     <row r="204" spans="1:10">
@@ -14016,7 +13935,7 @@
         <v>-0.04280312232530945</v>
       </c>
       <c r="J204">
-        <v>0.04732570251743054</v>
+        <v>0.04667257635058851</v>
       </c>
     </row>
     <row r="205" spans="1:10">
@@ -14048,7 +13967,7 @@
         <v>-0.01055551393951659</v>
       </c>
       <c r="J205">
-        <v>0.0466725763505885</v>
+        <v>0.04617623341781094</v>
       </c>
     </row>
     <row r="206" spans="1:10">
@@ -14080,7 +13999,7 @@
         <v>-0.0393647235222767</v>
       </c>
       <c r="J206">
-        <v>0.04617623341781093</v>
+        <v>0.04592129705949543</v>
       </c>
     </row>
     <row r="207" spans="1:10">
@@ -14112,7 +14031,7 @@
         <v>-0.04207277642190777</v>
       </c>
       <c r="J207">
-        <v>0.04592129705949543</v>
+        <v>0.04638902887860151</v>
       </c>
     </row>
     <row r="208" spans="1:10">
@@ -14144,7 +14063,7 @@
         <v>0.01931231103237288</v>
       </c>
       <c r="J208">
-        <v>0.0463890288786015</v>
+        <v>0.04393269502439472</v>
       </c>
     </row>
     <row r="209" spans="1:10">
@@ -14176,7 +14095,7 @@
         <v>-0.1121613668883301</v>
       </c>
       <c r="J209">
-        <v>0.04393269502439472</v>
+        <v>0.04734087531235841</v>
       </c>
     </row>
     <row r="210" spans="1:10">
@@ -14208,7 +14127,7 @@
         <v>-0.03635282946579827</v>
       </c>
       <c r="J210">
-        <v>0.0473408753123584</v>
+        <v>0.04748849550870715</v>
       </c>
     </row>
     <row r="211" spans="1:10">
@@ -14240,7 +14159,7 @@
         <v>0.0123237496888319</v>
       </c>
       <c r="J211">
-        <v>0.04748849550870714</v>
+        <v>0.04584518868454938</v>
       </c>
     </row>
     <row r="212" spans="1:10">
@@ -14272,7 +14191,7 @@
         <v>-0.016739324004298</v>
       </c>
       <c r="J212">
-        <v>0.04584518868454938</v>
+        <v>0.04561403356740665</v>
       </c>
     </row>
     <row r="213" spans="1:10">
@@ -14304,7 +14223,7 @@
         <v>0.03498096889524559</v>
       </c>
       <c r="J213">
-        <v>0.04561403356740663</v>
+        <v>0.04553807122006957</v>
       </c>
     </row>
     <row r="214" spans="1:10">
@@ -14336,7 +14255,7 @@
         <v>0.04879016416943204</v>
       </c>
       <c r="J214">
-        <v>0.04553807122006956</v>
+        <v>0.0469152248059188</v>
       </c>
     </row>
     <row r="215" spans="1:10">
@@ -14368,7 +14287,7 @@
         <v>-0.0874114570109695</v>
       </c>
       <c r="J215">
-        <v>0.0469152248059188</v>
+        <v>0.04872695075039508</v>
       </c>
     </row>
     <row r="216" spans="1:10">
@@ -14400,7 +14319,7 @@
         <v>-0.003104814953478756</v>
       </c>
       <c r="J216">
-        <v>0.04872695075039507</v>
+        <v>0.04801547165944649</v>
       </c>
     </row>
     <row r="217" spans="1:10">
@@ -14432,7 +14351,7 @@
         <v>-0.02316627803183959</v>
       </c>
       <c r="J217">
-        <v>0.04801547165944649</v>
+        <v>0.0465092901051298</v>
       </c>
     </row>
     <row r="218" spans="1:10">
@@ -14464,7 +14383,7 @@
         <v>0.04181350281341035</v>
       </c>
       <c r="J218">
-        <v>0.0465092901051298</v>
+        <v>0.0466039598783792</v>
       </c>
     </row>
     <row r="219" spans="1:10">
@@ -14496,7 +14415,7 @@
         <v>0.01882175424058767</v>
       </c>
       <c r="J219">
-        <v>0.0466039598783792</v>
+        <v>0.04690015528083764</v>
       </c>
     </row>
     <row r="220" spans="1:10">
@@ -14528,7 +14447,7 @@
         <v>-0.03759803041531849</v>
       </c>
       <c r="J220">
-        <v>0.04690015528083764</v>
+        <v>0.04655999875708907</v>
       </c>
     </row>
     <row r="221" spans="1:10">
@@ -14560,7 +14479,7 @@
         <v>0.01093994003833426</v>
       </c>
       <c r="J221">
-        <v>0.04655999875708907</v>
+        <v>0.04336390250510458</v>
       </c>
     </row>
     <row r="222" spans="1:10">
@@ -14592,7 +14511,7 @@
         <v>0.01508563741804095</v>
       </c>
       <c r="J222">
-        <v>0.04336390250510457</v>
+        <v>0.04316730727859661</v>
       </c>
     </row>
     <row r="223" spans="1:10">
@@ -14624,7 +14543,7 @@
         <v>0.1305895697036019</v>
       </c>
       <c r="J223">
-        <v>0.04316730727859661</v>
+        <v>0.05013214094344904</v>
       </c>
     </row>
     <row r="224" spans="1:10">
@@ -14656,7 +14575,7 @@
         <v>-0.003305457008726481</v>
       </c>
       <c r="J224">
-        <v>0.05013214094344903</v>
+        <v>0.04606100107029479</v>
       </c>
     </row>
     <row r="225" spans="1:10">
@@ -14688,7 +14607,7 @@
         <v>0.01469154874298968</v>
       </c>
       <c r="J225">
-        <v>0.04606100107029478</v>
+        <v>0.04612304871844301</v>
       </c>
     </row>
     <row r="226" spans="1:10">
@@ -14720,7 +14639,7 @@
         <v>0.04296369943211572</v>
       </c>
       <c r="J226">
-        <v>0.04612304871844301</v>
+        <v>0.04681785319413569</v>
       </c>
     </row>
     <row r="227" spans="1:10">
@@ -14752,7 +14671,7 @@
         <v>-0.03635282946579827</v>
       </c>
       <c r="J227">
-        <v>0.04681785319413569</v>
+        <v>0.04638610609690565</v>
       </c>
     </row>
     <row r="228" spans="1:10">
@@ -14784,7 +14703,7 @@
         <v>-0.02081513971392</v>
       </c>
       <c r="J228">
-        <v>0.04638610609690565</v>
+        <v>0.04582875675293629</v>
       </c>
     </row>
     <row r="229" spans="1:10">
@@ -14816,7 +14735,7 @@
         <v>0.03440142671733232</v>
       </c>
       <c r="J229">
-        <v>0.04582875675293629</v>
+        <v>0.04540285963203413</v>
       </c>
     </row>
     <row r="230" spans="1:10">
@@ -14848,7 +14767,7 @@
         <v>0.01291622526654623</v>
       </c>
       <c r="J230">
-        <v>0.04540285963203412</v>
+        <v>0.04498616430218414</v>
       </c>
     </row>
     <row r="231" spans="1:10">
@@ -14880,7 +14799,7 @@
         <v>0.06924617273681441</v>
       </c>
       <c r="J231">
-        <v>0.04498616430218414</v>
+        <v>0.04685354287642254</v>
       </c>
     </row>
     <row r="232" spans="1:10">
@@ -14912,7 +14831,7 @@
         <v>0.005982071677547469</v>
       </c>
       <c r="J232">
-        <v>0.04685354287642254</v>
+        <v>0.04668076166510614</v>
       </c>
     </row>
     <row r="233" spans="1:10">
@@ -14944,7 +14863,7 @@
         <v>-0.01349059018249914</v>
       </c>
       <c r="J233">
-        <v>0.04668076166510614</v>
+        <v>0.04655872237574905</v>
       </c>
     </row>
     <row r="234" spans="1:10">
@@ -14976,7 +14895,7 @@
         <v>0.01577491911536224</v>
       </c>
       <c r="J234">
-        <v>0.04655872237574905</v>
+        <v>0.04594398713700309</v>
       </c>
     </row>
     <row r="235" spans="1:10">
@@ -15008,7 +14927,7 @@
         <v>0.07584931228343783</v>
       </c>
       <c r="J235">
-        <v>0.0459439871370031</v>
+        <v>0.04782932744231107</v>
       </c>
     </row>
     <row r="236" spans="1:10">
@@ -15040,7 +14959,7 @@
         <v>-0.08272964759899602</v>
       </c>
       <c r="J236">
-        <v>0.04782932744231107</v>
+        <v>0.04981234278828056</v>
       </c>
     </row>
     <row r="237" spans="1:10">
@@ -15072,7 +14991,7 @@
         <v>0.04420825466432028</v>
       </c>
       <c r="J237">
-        <v>0.04981234278828058</v>
+        <v>0.04961226763530248</v>
       </c>
     </row>
     <row r="238" spans="1:10">
@@ -15104,7 +15023,7 @@
         <v>-0.03946874391036653</v>
       </c>
       <c r="J238">
-        <v>0.04961226763530249</v>
+        <v>0.05021923443371699</v>
       </c>
     </row>
     <row r="239" spans="1:10">
@@ -15136,7 +15055,7 @@
         <v>0.04659728537678226</v>
       </c>
       <c r="J239">
-        <v>0.050219234433717</v>
+        <v>0.04573281048851493</v>
       </c>
     </row>
     <row r="240" spans="1:10">
@@ -15168,7 +15087,7 @@
         <v>0.005683816468297709</v>
       </c>
       <c r="J240">
-        <v>0.04573281048851495</v>
+        <v>0.04492644398891828</v>
       </c>
     </row>
     <row r="241" spans="1:10">
@@ -15200,7 +15119,7 @@
         <v>-0.01704443460925847</v>
       </c>
       <c r="J241">
-        <v>0.04492644398891829</v>
+        <v>0.04520628843421672</v>
       </c>
     </row>
     <row r="242" spans="1:10">
@@ -15232,7 +15151,7 @@
         <v>-0.01887705576968918</v>
       </c>
       <c r="J242">
-        <v>0.04520628843421674</v>
+        <v>0.0452509069831117</v>
       </c>
     </row>
     <row r="243" spans="1:10">
@@ -15264,7 +15183,7 @@
         <v>0.01852730461388356</v>
       </c>
       <c r="J243">
-        <v>0.04525090698311171</v>
+        <v>0.04503100358021428</v>
       </c>
     </row>
     <row r="244" spans="1:10">
@@ -15296,7 +15215,7 @@
         <v>0.05534009503316455</v>
       </c>
       <c r="J244">
-        <v>0.04503100358021429</v>
+        <v>0.04524602281071509</v>
       </c>
     </row>
     <row r="245" spans="1:10">
@@ -15328,7 +15247,7 @@
         <v>-0.006118681008177177</v>
       </c>
       <c r="J245">
-        <v>0.0452460228107151</v>
+        <v>0.04154312694721237</v>
       </c>
     </row>
     <row r="246" spans="1:10">
@@ -15360,7 +15279,7 @@
         <v>0.01607018017749446</v>
       </c>
       <c r="J246">
-        <v>0.04154312694721238</v>
+        <v>0.04145152513758884</v>
       </c>
     </row>
     <row r="247" spans="1:10">
@@ -15392,7 +15311,7 @@
         <v>-0.02061095390412435</v>
       </c>
       <c r="J247">
-        <v>0.04145152513758886</v>
+        <v>0.04137816004744855</v>
       </c>
     </row>
     <row r="248" spans="1:10">
@@ -15424,7 +15343,7 @@
         <v>-0.03035612001489923</v>
       </c>
       <c r="J248">
-        <v>0.04137816004744856</v>
+        <v>0.04171985633383706</v>
       </c>
     </row>
     <row r="249" spans="1:10">
@@ -15456,7 +15375,7 @@
         <v>-0.01999864650668997</v>
       </c>
       <c r="J249">
-        <v>0.04171985633383708</v>
+        <v>0.04204497608063226</v>
       </c>
     </row>
     <row r="250" spans="1:10">
@@ -15488,7 +15407,7 @@
         <v>0.01439588028373234</v>
       </c>
       <c r="J250">
-        <v>0.04204497608063227</v>
+        <v>0.04112211806741883</v>
       </c>
     </row>
     <row r="251" spans="1:10">
@@ -15520,7 +15439,7 @@
         <v>-0.03262650282709417</v>
       </c>
       <c r="J251">
-        <v>0.04112211806741884</v>
+        <v>0.04187463279852702</v>
       </c>
     </row>
     <row r="252" spans="1:10">
@@ -15552,7 +15471,7 @@
         <v>-0.06956446338590916</v>
       </c>
       <c r="J252">
-        <v>0.04187463279852704</v>
+        <v>0.04425022487941449</v>
       </c>
     </row>
     <row r="253" spans="1:10">
@@ -15584,7 +15503,7 @@
         <v>0.005982071677547469</v>
       </c>
       <c r="J253">
-        <v>0.0442502248794145</v>
+        <v>0.03752835163917101</v>
       </c>
     </row>
     <row r="254" spans="1:10">
@@ -15616,7 +15535,7 @@
         <v>0.02576520788602642</v>
       </c>
       <c r="J254">
-        <v>0.03752835163917102</v>
+        <v>0.0377547958688868</v>
       </c>
     </row>
     <row r="255" spans="1:10">
@@ -15648,7 +15567,7 @@
         <v>-0.001501126126267091</v>
       </c>
       <c r="J255">
-        <v>0.0377547958688868</v>
+        <v>0.03770072136650984</v>
       </c>
     </row>
     <row r="256" spans="1:10">
@@ -15680,7 +15599,7 @@
         <v>-0.02367812735457715</v>
       </c>
       <c r="J256">
-        <v>0.03770072136650984</v>
+        <v>0.03720484248795761</v>
       </c>
     </row>
     <row r="257" spans="1:10">
@@ -15712,7 +15631,7 @@
         <v>-0.01562138090295678</v>
       </c>
       <c r="J257">
-        <v>0.03720484248795763</v>
+        <v>0.03668661013347918</v>
       </c>
     </row>
     <row r="258" spans="1:10">
@@ -15744,7 +15663,7 @@
         <v>-0.03469496979688685</v>
       </c>
       <c r="J258">
-        <v>0.03668661013347919</v>
+        <v>0.0370586880784157</v>
       </c>
     </row>
     <row r="259" spans="1:10">
@@ -15776,7 +15695,7 @@
         <v>0.02293497128249599</v>
       </c>
       <c r="J259">
-        <v>0.03705868807841571</v>
+        <v>0.03675678659575884</v>
       </c>
     </row>
     <row r="260" spans="1:10">
@@ -15808,7 +15727,7 @@
         <v>-0.0008003201707691552</v>
       </c>
       <c r="J260">
-        <v>0.03675678659575885</v>
+        <v>0.03667962467037262</v>
       </c>
     </row>
     <row r="261" spans="1:10">
@@ -15840,7 +15759,7 @@
         <v>0.03478782548566402</v>
       </c>
       <c r="J261">
-        <v>0.03667962467037262</v>
+        <v>0.03492896728285341</v>
       </c>
     </row>
     <row r="262" spans="1:10">
@@ -15872,7 +15791,7 @@
         <v>-0.01541825272838064</v>
       </c>
       <c r="J262">
-        <v>0.03492896728285343</v>
+        <v>0.03499338729032145</v>
       </c>
     </row>
     <row r="263" spans="1:10">
@@ -15904,7 +15823,7 @@
         <v>-0.05087233037375655</v>
       </c>
       <c r="J263">
-        <v>0.03499338729032146</v>
+        <v>0.03606496380671797</v>
       </c>
     </row>
     <row r="264" spans="1:10">
@@ -15936,7 +15855,7 @@
         <v>-0.06240746012861705</v>
       </c>
       <c r="J264">
-        <v>0.03606496380671798</v>
+        <v>0.03743994359838088</v>
       </c>
     </row>
     <row r="265" spans="1:10">
@@ -15968,7 +15887,7 @@
         <v>0.01084102317787477</v>
       </c>
       <c r="J265">
-        <v>0.03743994359838089</v>
+        <v>0.03429609298679161</v>
       </c>
     </row>
     <row r="266" spans="1:10">
@@ -16000,7 +15919,7 @@
         <v>-0.01582455034697146</v>
       </c>
       <c r="J266">
-        <v>0.03429609298679163</v>
+        <v>0.03131790857224283</v>
       </c>
     </row>
     <row r="267" spans="1:10">
@@ -16032,7 +15951,7 @@
         <v>-0.01724789340955339</v>
       </c>
       <c r="J267">
-        <v>0.03131790857224284</v>
+        <v>0.02991161069059445</v>
       </c>
     </row>
     <row r="268" spans="1:10">
@@ -16064,7 +15983,7 @@
         <v>0.001299155731620129</v>
       </c>
       <c r="J268">
-        <v>0.02991161069059447</v>
+        <v>0.02934681040834167</v>
       </c>
     </row>
     <row r="269" spans="1:10">
@@ -16096,7 +16015,7 @@
         <v>-0.03345337625921958</v>
       </c>
       <c r="J269">
-        <v>0.02934681040834168</v>
+        <v>0.02795882262095474</v>
       </c>
     </row>
     <row r="270" spans="1:10">
@@ -16128,7 +16047,7 @@
         <v>0.04974209189481401</v>
       </c>
       <c r="J270">
-        <v>0.02795882262095475</v>
+        <v>0.02985853973205195</v>
       </c>
     </row>
     <row r="271" spans="1:10">
@@ -16160,7 +16079,7 @@
         <v>-0.0114654781092781</v>
       </c>
       <c r="J271">
-        <v>0.02985853973205197</v>
+        <v>0.02981568309723496</v>
       </c>
     </row>
     <row r="272" spans="1:10">
@@ -16192,7 +16111,7 @@
         <v>0.01488861249375056</v>
       </c>
       <c r="J272">
-        <v>0.02981568309723497</v>
+        <v>0.03000867665558427</v>
       </c>
     </row>
     <row r="273" spans="1:10">
@@ -16224,7 +16143,7 @@
         <v>0.004688989486131469</v>
       </c>
       <c r="J273">
-        <v>0.03000867665558428</v>
+        <v>0.02971740516507494</v>
       </c>
     </row>
     <row r="274" spans="1:10">
@@ -16256,7 +16175,7 @@
         <v>0.01547957084838637</v>
       </c>
       <c r="J274">
-        <v>0.02971740516507495</v>
+        <v>0.02766086212314196</v>
       </c>
     </row>
     <row r="275" spans="1:10">
@@ -16288,7 +16207,7 @@
         <v>0.0104452578615386</v>
       </c>
       <c r="J275">
-        <v>0.02766086212314197</v>
+        <v>0.02786795510380945</v>
       </c>
     </row>
     <row r="276" spans="1:10">
@@ -16320,7 +16239,7 @@
         <v>-0.03025304317102094</v>
       </c>
       <c r="J276">
-        <v>0.02786795510380946</v>
+        <v>0.02779288165683477</v>
       </c>
     </row>
     <row r="277" spans="1:10">
@@ -16352,7 +16271,7 @@
         <v>0.01764343517259528</v>
       </c>
       <c r="J277">
-        <v>0.02779288165683478</v>
+        <v>0.0281255080340488</v>
       </c>
     </row>
     <row r="278" spans="1:10">
@@ -16384,7 +16303,7 @@
         <v>0.004191204618468052</v>
       </c>
       <c r="J278">
-        <v>0.02812550803404881</v>
+        <v>0.02788038760594146</v>
       </c>
     </row>
     <row r="279" spans="1:10">
@@ -16416,7 +16335,7 @@
         <v>0.004589452333807224</v>
       </c>
       <c r="J279">
-        <v>0.02788038760594148</v>
+        <v>0.02783870442917118</v>
       </c>
     </row>
     <row r="280" spans="1:10">
@@ -16448,7 +16367,7 @@
         <v>-0.00964637705180545</v>
       </c>
       <c r="J280">
-        <v>0.02783870442917119</v>
+        <v>0.02757838109601</v>
       </c>
     </row>
     <row r="281" spans="1:10">
@@ -16480,7 +16399,7 @@
         <v>-0.01541825272838064</v>
       </c>
       <c r="J281">
-        <v>0.02757838109601001</v>
+        <v>0.02719743502125063</v>
       </c>
     </row>
     <row r="282" spans="1:10">
@@ -16512,7 +16431,7 @@
         <v>-0.1041390397411454</v>
       </c>
       <c r="J282">
-        <v>0.02719743502125065</v>
+        <v>0.03050817903233894</v>
       </c>
     </row>
     <row r="283" spans="1:10">
@@ -16544,7 +16463,7 @@
         <v>0.01705375456582762</v>
       </c>
       <c r="J283">
-        <v>0.03050817903233895</v>
+        <v>0.03074054208453561</v>
       </c>
     </row>
     <row r="284" spans="1:10">
@@ -16576,7 +16495,7 @@
         <v>-0.04908520769049141</v>
       </c>
       <c r="J284">
-        <v>0.03074054208453561</v>
+        <v>0.03103103217415878</v>
       </c>
     </row>
     <row r="285" spans="1:10">
@@ -16608,7 +16527,7 @@
         <v>-0.03874082831643059</v>
       </c>
       <c r="J285">
-        <v>0.0310310321741588</v>
+        <v>0.03144494422438562</v>
       </c>
     </row>
     <row r="286" spans="1:10">
@@ -16640,7 +16559,7 @@
         <v>0.05240267879304842</v>
       </c>
       <c r="J286">
-        <v>0.03144494422438563</v>
+        <v>0.03336897849963345</v>
       </c>
     </row>
     <row r="287" spans="1:10">
@@ -16672,7 +16591,7 @@
         <v>-0.03822121282019774</v>
       </c>
       <c r="J287">
-        <v>0.03336897849963346</v>
+        <v>0.03379614640165492</v>
       </c>
     </row>
     <row r="288" spans="1:10">
@@ -16704,7 +16623,7 @@
         <v>0.01567647938500762</v>
       </c>
       <c r="J288">
-        <v>0.03379614640165493</v>
+        <v>0.0337210908596999</v>
       </c>
     </row>
     <row r="289" spans="1:10">
@@ -16736,7 +16655,7 @@
         <v>-0.007729798061941268</v>
       </c>
       <c r="J289">
-        <v>0.03372109085969992</v>
+        <v>0.03323707640521417</v>
       </c>
     </row>
     <row r="290" spans="1:10">
@@ -16768,7 +16687,7 @@
         <v>0.04162167469081945</v>
       </c>
       <c r="J290">
-        <v>0.03323707640521419</v>
+        <v>0.03444468905953855</v>
       </c>
     </row>
     <row r="291" spans="1:10">
@@ -16800,7 +16719,7 @@
         <v>0.004191204618468052</v>
       </c>
       <c r="J291">
-        <v>0.03444468905953856</v>
+        <v>0.03361318975286033</v>
       </c>
     </row>
     <row r="292" spans="1:10">
@@ -16832,7 +16751,7 @@
         <v>0.003394233068015617</v>
       </c>
       <c r="J292">
-        <v>0.03361318975286035</v>
+        <v>0.03364238441221256</v>
       </c>
     </row>
     <row r="293" spans="1:10">
@@ -16864,7 +16783,7 @@
         <v>-0.006923915072824198</v>
       </c>
       <c r="J293">
-        <v>0.03364238441221257</v>
+        <v>0.03261687507160303</v>
       </c>
     </row>
     <row r="294" spans="1:10">
@@ -16896,7 +16815,7 @@
         <v>-0.1052494107190975</v>
       </c>
       <c r="J294">
-        <v>0.03261687507160305</v>
+        <v>0.03595068622615863</v>
       </c>
     </row>
     <row r="295" spans="1:10">
@@ -16928,7 +16847,7 @@
         <v>0.017938145131013</v>
       </c>
       <c r="J295">
-        <v>0.03595068622615864</v>
+        <v>0.03609638302339636</v>
       </c>
     </row>
     <row r="296" spans="1:10">
@@ -16960,7 +16879,7 @@
         <v>-0.0006001800720324606</v>
       </c>
       <c r="J296">
-        <v>0.03609638302339637</v>
+        <v>0.03607415777626211</v>
       </c>
     </row>
     <row r="297" spans="1:10">
@@ -16992,7 +16911,7 @@
         <v>0.01587334915629016</v>
       </c>
       <c r="J297">
-        <v>0.03607415777626213</v>
+        <v>0.03623815299745176</v>
       </c>
     </row>
     <row r="298" spans="1:10">
@@ -17024,7 +16943,7 @@
         <v>-0.02726842715419378</v>
       </c>
       <c r="J298">
-        <v>0.03623815299745178</v>
+        <v>0.03643285321620724</v>
       </c>
     </row>
     <row r="299" spans="1:10">
@@ -17056,7 +16975,7 @@
         <v>0.008959741371471801</v>
       </c>
       <c r="J299">
-        <v>0.03643285321620725</v>
+        <v>0.03616392448165148</v>
       </c>
     </row>
     <row r="300" spans="1:10">
@@ -17088,7 +17007,7 @@
         <v>-0.0473012731180131</v>
       </c>
       <c r="J300">
-        <v>0.03616392448165149</v>
+        <v>0.03544396718099081</v>
       </c>
     </row>
     <row r="301" spans="1:10">
@@ -17120,7 +17039,7 @@
         <v>0.05940034328144746</v>
       </c>
       <c r="J301">
-        <v>0.03544396718099083</v>
+        <v>0.03751301501587786</v>
       </c>
     </row>
     <row r="302" spans="1:10">
@@ -17152,7 +17071,7 @@
         <v>0.02907324748570717</v>
       </c>
       <c r="J302">
-        <v>0.03751301501587787</v>
+        <v>0.03786965871599138</v>
       </c>
     </row>
     <row r="303" spans="1:10">
@@ -17184,7 +17103,7 @@
         <v>-0.006521216990265463</v>
       </c>
       <c r="J303">
-        <v>0.03786965871599138</v>
+        <v>0.03782333003892257</v>
       </c>
     </row>
     <row r="304" spans="1:10">
@@ -17216,7 +17135,7 @@
         <v>0.0358496528936972</v>
       </c>
       <c r="J304">
-        <v>0.03782333003892259</v>
+        <v>0.03839405481716213</v>
       </c>
     </row>
     <row r="305" spans="1:10">
@@ -17248,7 +17167,7 @@
         <v>-0.01247752151111258</v>
       </c>
       <c r="J305">
-        <v>0.03839405481716214</v>
+        <v>0.0383048950747691</v>
       </c>
     </row>
     <row r="306" spans="1:10">
@@ -17280,7 +17199,7 @@
         <v>0.01370564705611197</v>
       </c>
       <c r="J306">
-        <v>0.03830489507476911</v>
+        <v>0.03817478006110021</v>
       </c>
     </row>
     <row r="307" spans="1:10">
@@ -17312,7 +17231,7 @@
         <v>-0.007629027164491163</v>
       </c>
       <c r="J307">
-        <v>0.03817478006110023</v>
+        <v>0.03795299777729269</v>
       </c>
     </row>
     <row r="308" spans="1:10">
@@ -17344,7 +17263,7 @@
         <v>0.009455158770755197</v>
       </c>
       <c r="J308">
-        <v>0.03795299777729271</v>
+        <v>0.03800956527887916</v>
       </c>
     </row>
     <row r="309" spans="1:10">
@@ -17376,7 +17295,7 @@
         <v>0.02391182004631288</v>
       </c>
       <c r="J309">
-        <v>0.03800956527887917</v>
+        <v>0.0383386446742174</v>
       </c>
     </row>
     <row r="310" spans="1:10">
@@ -17408,7 +17327,7 @@
         <v>-0.008132983230188991</v>
       </c>
       <c r="J310">
-        <v>0.03833864467421742</v>
+        <v>0.03833233721543892</v>
       </c>
     </row>
     <row r="311" spans="1:10">
@@ -17440,7 +17359,7 @@
         <v>-0.006018072325563021</v>
       </c>
       <c r="J311">
-        <v>0.03833233721543894</v>
+        <v>0.03827611504380398</v>
       </c>
     </row>
     <row r="312" spans="1:10">
@@ -17472,7 +17391,7 @@
         <v>-0.05635873366938424</v>
       </c>
       <c r="J312">
-        <v>0.038276115043804</v>
+        <v>0.03479814448832069</v>
       </c>
     </row>
     <row r="313" spans="1:10">
@@ -17504,7 +17423,7 @@
         <v>0.01202738021271845</v>
       </c>
       <c r="J313">
-        <v>0.03479814448832071</v>
+        <v>0.03471362012797393</v>
       </c>
     </row>
     <row r="314" spans="1:10">
@@ -17536,7 +17455,7 @@
         <v>-0.02040680977766262</v>
       </c>
       <c r="J314">
-        <v>0.03471362012797394</v>
+        <v>0.03376830703505167</v>
       </c>
     </row>
     <row r="315" spans="1:10">
@@ -17568,7 +17487,7 @@
         <v>-0.004610612557683294</v>
       </c>
       <c r="J315">
-        <v>0.03376830703505169</v>
+        <v>0.03303870542200151</v>
       </c>
     </row>
     <row r="316" spans="1:10">
@@ -17600,7 +17519,7 @@
         <v>0.004788516731797094</v>
       </c>
       <c r="J316">
-        <v>0.03303870542200153</v>
+        <v>0.03152363828212815</v>
       </c>
     </row>
     <row r="317" spans="1:10">
@@ -17632,7 +17551,7 @@
         <v>0.01538110203830239</v>
       </c>
       <c r="J317">
-        <v>0.03152363828212817</v>
+        <v>0.03091217515848833</v>
       </c>
     </row>
     <row r="318" spans="1:10">
@@ -17664,7 +17583,7 @@
         <v>0.05845756957156869</v>
       </c>
       <c r="J318">
-        <v>0.03091217515848834</v>
+        <v>0.03260997249189732</v>
       </c>
     </row>
     <row r="319" spans="1:10">
@@ -17696,7 +17615,7 @@
         <v>0.08415730800672341</v>
       </c>
       <c r="J319">
-        <v>0.03260997249189733</v>
+        <v>0.03589002628379434</v>
       </c>
     </row>
     <row r="320" spans="1:10">
@@ -17728,7 +17647,7 @@
         <v>0.008067371077758793</v>
       </c>
       <c r="J320">
-        <v>0.03589002628379435</v>
+        <v>0.03520275432855542</v>
       </c>
     </row>
     <row r="321" spans="1:10">
@@ -17760,7 +17679,7 @@
         <v>0.01271877240777461</v>
       </c>
       <c r="J321">
-        <v>0.03520275432855544</v>
+        <v>0.03524567792851206</v>
       </c>
     </row>
     <row r="322" spans="1:10">
@@ -17792,7 +17711,7 @@
         <v>-0.01897896659780286</v>
       </c>
       <c r="J322">
-        <v>0.03524567792851207</v>
+        <v>0.03548291821366509</v>
       </c>
     </row>
     <row r="323" spans="1:10">
@@ -17824,7 +17743,7 @@
         <v>0.009554212804811711</v>
       </c>
       <c r="J323">
-        <v>0.0354829182136651</v>
+        <v>0.03545617997107978</v>
       </c>
     </row>
     <row r="324" spans="1:10">
@@ -17856,7 +17775,7 @@
         <v>-0.0004000800213396913</v>
       </c>
       <c r="J324">
-        <v>0.0354561799710798</v>
+        <v>0.02896488663947568</v>
       </c>
     </row>
     <row r="325" spans="1:10">
@@ -17888,7 +17807,7 @@
         <v>0.04219704869978828</v>
       </c>
       <c r="J325">
-        <v>0.0289648866394757</v>
+        <v>0.02961912859697697</v>
       </c>
     </row>
     <row r="326" spans="1:10">
@@ -17920,7 +17839,7 @@
         <v>0.08378952572968316</v>
       </c>
       <c r="J326">
-        <v>0.02961912859697698</v>
+        <v>0.0326676244900788</v>
       </c>
     </row>
     <row r="327" spans="1:10">
@@ -17952,7 +17871,7 @@
         <v>-0.02634397533960198</v>
       </c>
       <c r="J327">
-        <v>0.03266762449007882</v>
+        <v>0.03332531281537623</v>
       </c>
     </row>
     <row r="328" spans="1:10">
@@ -17984,7 +17903,7 @@
         <v>-0.02942881069081217</v>
       </c>
       <c r="J328">
-        <v>0.03332531281537624</v>
+        <v>0.0334085471016218</v>
       </c>
     </row>
     <row r="329" spans="1:10">
@@ -18016,7 +17935,7 @@
         <v>0.03062619354176075</v>
       </c>
       <c r="J329">
-        <v>0.03340854710162181</v>
+        <v>0.03364333198428136</v>
       </c>
     </row>
     <row r="330" spans="1:10">
@@ -18048,7 +17967,7 @@
         <v>0.007372754329413157</v>
       </c>
       <c r="J330">
-        <v>0.03364333198428138</v>
+        <v>0.03188875547537803</v>
       </c>
     </row>
     <row r="331" spans="1:10">
@@ -18080,7 +17999,7 @@
         <v>-0.003104814953478756</v>
       </c>
       <c r="J331">
-        <v>0.03188875547537805</v>
+        <v>0.03066567668637943</v>
       </c>
     </row>
     <row r="332" spans="1:10">
@@ -18112,7 +18031,7 @@
         <v>-0.005012541823544286</v>
       </c>
       <c r="J332">
-        <v>0.03066567668637945</v>
+        <v>0.03054119876804298</v>
       </c>
     </row>
     <row r="333" spans="1:10">
@@ -18144,7 +18063,7 @@
         <v>-0.05646453698112658</v>
       </c>
       <c r="J333">
-        <v>0.03054119876804299</v>
+        <v>0.03266018381843179</v>
       </c>
     </row>
     <row r="334" spans="1:10">
@@ -18176,7 +18095,7 @@
         <v>-0.01592615055025925</v>
       </c>
       <c r="J334">
-        <v>0.03266018381843181</v>
+        <v>0.03242601930638046</v>
       </c>
     </row>
     <row r="335" spans="1:10">
@@ -18208,7 +18127,7 @@
         <v>-0.009747351454880074</v>
       </c>
       <c r="J335">
-        <v>0.03242601930638047</v>
+        <v>0.03237956596998736</v>
       </c>
     </row>
     <row r="336" spans="1:10">
@@ -18240,7 +18159,7 @@
         <v>-0.01541825272838064</v>
       </c>
       <c r="J336">
-        <v>0.03237956596998737</v>
+        <v>0.03254330118719578</v>
       </c>
     </row>
     <row r="337" spans="1:10">
@@ -18272,7 +18191,7 @@
         <v>-0.05635873366938424</v>
       </c>
       <c r="J337">
-        <v>0.0325433011871958</v>
+        <v>0.03430940283011538</v>
       </c>
     </row>
     <row r="338" spans="1:10">
@@ -18304,7 +18223,7 @@
         <v>0.001798381941379397</v>
       </c>
       <c r="J338">
-        <v>0.0343094028301154</v>
+        <v>0.03428301309305826</v>
       </c>
     </row>
     <row r="339" spans="1:10">
@@ -18336,7 +18255,7 @@
         <v>-0.01207258123426925</v>
       </c>
       <c r="J339">
-        <v>0.03428301309305827</v>
+        <v>0.03412163697266186</v>
       </c>
     </row>
     <row r="340" spans="1:10">
@@ -18368,7 +18287,7 @@
         <v>-0.03231660147654312</v>
       </c>
       <c r="J340">
-        <v>0.03412163697266188</v>
+        <v>0.03462368290730836</v>
       </c>
     </row>
     <row r="341" spans="1:10">
@@ -18400,7 +18319,7 @@
         <v>-0.06795769318322709</v>
       </c>
       <c r="J341">
-        <v>0.03462368290730837</v>
+        <v>0.03677867574343319</v>
       </c>
     </row>
     <row r="342" spans="1:10">
@@ -18432,7 +18351,7 @@
         <v>0.0390283869674784</v>
       </c>
       <c r="J342">
-        <v>0.03677867574343321</v>
+        <v>0.03603276358422119</v>
       </c>
     </row>
     <row r="343" spans="1:10">
@@ -18464,7 +18383,7 @@
         <v>-0.06038715001509513</v>
       </c>
       <c r="J343">
-        <v>0.0360327635842212</v>
+        <v>0.03766942033364431</v>
       </c>
     </row>
     <row r="344" spans="1:10">
@@ -18496,7 +18415,7 @@
         <v>0.01390290516899143</v>
       </c>
       <c r="J344">
-        <v>0.03766942033364432</v>
+        <v>0.03758797184655507</v>
       </c>
     </row>
     <row r="345" spans="1:10">
@@ -18528,7 +18447,7 @@
         <v>0.01291622526654623</v>
       </c>
       <c r="J345">
-        <v>0.03758797184655508</v>
+        <v>0.03765143510866008</v>
       </c>
     </row>
     <row r="346" spans="1:10">
@@ -18560,7 +18479,7 @@
         <v>-0.009848336054814406</v>
       </c>
       <c r="J346">
-        <v>0.03765143510866009</v>
+        <v>0.0376886902435454</v>
       </c>
     </row>
     <row r="347" spans="1:10">
@@ -18592,7 +18511,7 @@
         <v>-0.01015135105637536</v>
       </c>
       <c r="J347">
-        <v>0.03768869024354541</v>
+        <v>0.03761775427380053</v>
       </c>
     </row>
     <row r="348" spans="1:10">
@@ -18624,7 +18543,7 @@
         <v>0.01301493707749476</v>
       </c>
       <c r="J348">
-        <v>0.03761775427380053</v>
+        <v>0.03602886441831785</v>
       </c>
     </row>
     <row r="349" spans="1:10">
@@ -18656,7 +18575,7 @@
         <v>0.006975613736425138</v>
       </c>
       <c r="J349">
-        <v>0.03602886441831787</v>
+        <v>0.03218897289574918</v>
       </c>
     </row>
     <row r="350" spans="1:10">
@@ -18688,7 +18607,7 @@
         <v>0.04181350281341035</v>
       </c>
       <c r="J350">
-        <v>0.03218897289574919</v>
+        <v>0.03323166216823164</v>
       </c>
     </row>
     <row r="351" spans="1:10">
@@ -18720,7 +18639,7 @@
         <v>-0.02963480512969074</v>
       </c>
       <c r="J351">
-        <v>0.03323166216823165</v>
+        <v>0.03340459364819545</v>
       </c>
     </row>
     <row r="352" spans="1:10">
@@ -18752,7 +18671,7 @@
         <v>0.01459300230290009</v>
       </c>
       <c r="J352">
-        <v>0.03340459364819547</v>
+        <v>0.03348995391246683</v>
       </c>
     </row>
     <row r="353" spans="1:10">
@@ -18784,7 +18703,7 @@
         <v>-0.03593810680562915</v>
       </c>
       <c r="J353">
-        <v>0.03348995391246685</v>
+        <v>0.03387807902952664</v>
       </c>
     </row>
     <row r="354" spans="1:10">
@@ -18816,7 +18735,7 @@
         <v>0.03507752661269616</v>
       </c>
       <c r="J354">
-        <v>0.03387807902952665</v>
+        <v>0.03467624293021392</v>
       </c>
     </row>
     <row r="355" spans="1:10">
@@ -18848,7 +18767,7 @@
         <v>-0.01938671380019009</v>
       </c>
       <c r="J355">
-        <v>0.03467624293021393</v>
+        <v>0.03362756541709649</v>
       </c>
     </row>
     <row r="356" spans="1:10">
@@ -18880,7 +18799,7 @@
         <v>0.02673929718962151</v>
       </c>
       <c r="J356">
-        <v>0.03362756541709651</v>
+        <v>0.02973405343004509</v>
       </c>
     </row>
     <row r="357" spans="1:10">
@@ -18912,7 +18831,7 @@
         <v>0.02547279597303107</v>
       </c>
       <c r="J357">
-        <v>0.0297340534300451</v>
+        <v>0.03015702611673006</v>
       </c>
     </row>
     <row r="358" spans="1:10">
@@ -18944,7 +18863,7 @@
         <v>0.005484930230569745</v>
       </c>
       <c r="J358">
-        <v>0.03015702611673008</v>
+        <v>0.02992083943158552</v>
       </c>
     </row>
     <row r="359" spans="1:10">
@@ -18976,7 +18895,7 @@
         <v>-0.003606495594111744</v>
       </c>
       <c r="J359">
-        <v>0.02992083943158553</v>
+        <v>0.02913823790374747</v>
       </c>
     </row>
     <row r="360" spans="1:10">
@@ -19008,7 +18927,7 @@
         <v>0.02955880224154443</v>
       </c>
       <c r="J360">
-        <v>0.02913823790374748</v>
+        <v>0.02978056131135114</v>
       </c>
     </row>
     <row r="361" spans="1:10">
@@ -19040,7 +18959,7 @@
         <v>0.02430229252296482</v>
       </c>
       <c r="J361">
-        <v>0.02978056131135116</v>
+        <v>0.03028532116518527</v>
       </c>
     </row>
     <row r="362" spans="1:10">
@@ -19072,7 +18991,7 @@
         <v>-0.004811556997222082</v>
       </c>
       <c r="J362">
-        <v>0.03028532116518529</v>
+        <v>0.03028533708353798</v>
       </c>
     </row>
     <row r="363" spans="1:10">
@@ -19104,7 +19023,7 @@
         <v>-0.007226045091739582</v>
       </c>
       <c r="J363">
-        <v>0.030285337083538</v>
+        <v>0.02869113115285059</v>
       </c>
     </row>
     <row r="364" spans="1:10">
@@ -19136,7 +19055,7 @@
         <v>0.004489905272852001</v>
       </c>
       <c r="J364">
-        <v>0.02869113115285061</v>
+        <v>0.0286242772347444</v>
       </c>
     </row>
     <row r="365" spans="1:10">
@@ -19168,7 +19087,7 @@
         <v>0.0241070753432331</v>
       </c>
       <c r="J365">
-        <v>0.02862427723474442</v>
+        <v>0.0289999577759959</v>
       </c>
     </row>
     <row r="366" spans="1:10">
@@ -19200,7 +19119,7 @@
         <v>0.01281750371061434</v>
       </c>
       <c r="J366">
-        <v>0.02899995777599592</v>
+        <v>0.02899179782398455</v>
       </c>
     </row>
     <row r="367" spans="1:10">
@@ -19232,7 +19151,7 @@
         <v>-0.003104814953478756</v>
       </c>
       <c r="J367">
-        <v>0.02899179782398456</v>
+        <v>0.02702266085904973</v>
       </c>
     </row>
     <row r="368" spans="1:10">
@@ -19264,7 +19183,7 @@
         <v>0.01242251999855711</v>
       </c>
       <c r="J368">
-        <v>0.02702266085904975</v>
+        <v>0.02710043490402003</v>
       </c>
     </row>
     <row r="369" spans="1:10">
@@ -19296,7 +19215,7 @@
         <v>-0.09222494404251728</v>
       </c>
       <c r="J369">
-        <v>0.02710043490402006</v>
+        <v>0.03199751598619492</v>
       </c>
     </row>
     <row r="370" spans="1:10">
@@ -19328,7 +19247,7 @@
         <v>-0.02942881069081217</v>
       </c>
       <c r="J370">
-        <v>0.03199751598619494</v>
+        <v>0.03190466731275978</v>
       </c>
     </row>
     <row r="371" spans="1:10">
@@ -19360,7 +19279,7 @@
         <v>-0.01724789340955339</v>
       </c>
       <c r="J371">
-        <v>0.0319046673127598</v>
+        <v>0.02948852309128277</v>
       </c>
     </row>
     <row r="372" spans="1:10">
@@ -19392,7 +19311,7 @@
         <v>-0.03479850554269554</v>
       </c>
       <c r="J372">
-        <v>0.02948852309128279</v>
+        <v>0.02925554249026528</v>
       </c>
     </row>
     <row r="373" spans="1:10">
@@ -19424,7 +19343,7 @@
         <v>0.008860628432196467</v>
       </c>
       <c r="J373">
-        <v>0.0292555424902653</v>
+        <v>0.02712840590629908</v>
       </c>
     </row>
     <row r="374" spans="1:10">
@@ -19456,7 +19375,7 @@
         <v>0.01084102317787477</v>
       </c>
       <c r="J374">
-        <v>0.0271284059062991</v>
+        <v>0.02708198089825377</v>
       </c>
     </row>
     <row r="375" spans="1:10">
@@ -19488,7 +19407,7 @@
         <v>-0.002703651574314823</v>
       </c>
       <c r="J375">
-        <v>0.02708198089825379</v>
+        <v>0.02698307486166235</v>
       </c>
     </row>
     <row r="376" spans="1:10">
@@ -19520,7 +19439,7 @@
         <v>0.006478966097709074</v>
       </c>
       <c r="J376">
-        <v>0.02698307486166238</v>
+        <v>0.02694468073019</v>
       </c>
     </row>
     <row r="377" spans="1:10">
@@ -19552,7 +19471,7 @@
         <v>0.02244618882983</v>
       </c>
       <c r="J377">
-        <v>0.02694468073019002</v>
+        <v>0.0271598288171204</v>
       </c>
     </row>
     <row r="378" spans="1:10">
@@ -19584,7 +19503,7 @@
         <v>0.001498876123735949</v>
       </c>
       <c r="J378">
-        <v>0.02715982881712042</v>
+        <v>0.02707289855569762</v>
       </c>
     </row>
     <row r="379" spans="1:10">
@@ -19616,7 +19535,7 @@
         <v>0.004390348301292854</v>
       </c>
       <c r="J379">
-        <v>0.02707289855569764</v>
+        <v>0.0270577566402723</v>
       </c>
     </row>
     <row r="380" spans="1:10">
@@ -19648,7 +19567,7 @@
         <v>-0.002302649062675558</v>
       </c>
       <c r="J380">
-        <v>0.02705775664027232</v>
+        <v>0.02594131809915814</v>
       </c>
     </row>
     <row r="381" spans="1:10">
@@ -19680,7 +19599,7 @@
         <v>-0.03832511432166789</v>
       </c>
       <c r="J381">
-        <v>0.02594131809915817</v>
+        <v>0.02632440054540878</v>
       </c>
     </row>
     <row r="382" spans="1:10">
@@ -19712,7 +19631,7 @@
         <v>0.01410012437878163</v>
       </c>
       <c r="J382">
-        <v>0.02632440054540881</v>
+        <v>0.02631466767949188</v>
       </c>
     </row>
     <row r="383" spans="1:10">
@@ -19744,7 +19663,7 @@
         <v>0.007571265496318126</v>
       </c>
       <c r="J383">
-        <v>0.0263146676794919</v>
+        <v>0.02549369514630842</v>
       </c>
     </row>
     <row r="384" spans="1:10">
@@ -19776,7 +19695,7 @@
         <v>0.01695544064941337</v>
       </c>
       <c r="J384">
-        <v>0.02549369514630844</v>
+        <v>0.02485821847740991</v>
       </c>
     </row>
     <row r="385" spans="1:10">
@@ -19808,7 +19727,7 @@
         <v>0.03950913309471249</v>
       </c>
       <c r="J385">
-        <v>0.02485821847740994</v>
+        <v>0.02558034510769616</v>
       </c>
     </row>
     <row r="386" spans="1:10">
@@ -19840,7 +19759,7 @@
         <v>-0.005917473764037623</v>
       </c>
       <c r="J386">
-        <v>0.02558034510769619</v>
+        <v>0.02518641334279012</v>
       </c>
     </row>
     <row r="387" spans="1:10">
@@ -19872,7 +19791,7 @@
         <v>-0.001901807289596331</v>
       </c>
       <c r="J387">
-        <v>0.02518641334279014</v>
+        <v>0.02476100861973104</v>
       </c>
     </row>
     <row r="388" spans="1:10">
@@ -19904,7 +19823,7 @@
         <v>-0.01877515532633398</v>
       </c>
       <c r="J388">
-        <v>0.02476100861973107</v>
+        <v>0.02497346016799002</v>
       </c>
     </row>
     <row r="389" spans="1:10">
@@ -19936,7 +19855,7 @@
         <v>-0.02306393959855169</v>
       </c>
       <c r="J389">
-        <v>0.02497346016799005</v>
+        <v>0.02530114257101593</v>
       </c>
     </row>
     <row r="390" spans="1:10">
@@ -19968,7 +19887,7 @@
         <v>0.004290781417156246</v>
       </c>
       <c r="J390">
-        <v>0.02530114257101596</v>
+        <v>0.02464773467369615</v>
       </c>
     </row>
     <row r="391" spans="1:10">
@@ -20000,7 +19919,7 @@
         <v>0.03498096889524559</v>
       </c>
       <c r="J391">
-        <v>0.02464773467369617</v>
+        <v>0.02511669307014433</v>
       </c>
     </row>
     <row r="392" spans="1:10">
@@ -20032,7 +19951,7 @@
         <v>-0.008637193395663588</v>
       </c>
       <c r="J392">
-        <v>0.02511669307014435</v>
+        <v>0.02514184682524425</v>
       </c>
     </row>
     <row r="393" spans="1:10">
@@ -20064,7 +19983,7 @@
         <v>-0.004610612557683294</v>
       </c>
       <c r="J393">
-        <v>0.02514184682524428</v>
+        <v>0.02512761855299769</v>
       </c>
     </row>
     <row r="394" spans="1:10">
@@ -20096,7 +20015,7 @@
         <v>0.001998002662673058</v>
       </c>
       <c r="J394">
-        <v>0.02512761855299771</v>
+        <v>0.02510984759587818</v>
       </c>
     </row>
     <row r="395" spans="1:10">
@@ -20128,7 +20047,7 @@
         <v>-0.002402884616310315</v>
       </c>
       <c r="J395">
-        <v>0.0251098475958782</v>
+        <v>0.02462139933858899</v>
       </c>
     </row>
     <row r="396" spans="1:10">
@@ -20160,7 +20079,7 @@
         <v>-0.01045445790385887</v>
       </c>
       <c r="J396">
-        <v>0.02462139933858902</v>
+        <v>0.02447607861564224</v>
       </c>
     </row>
     <row r="397" spans="1:10">
@@ -20192,7 +20111,7 @@
         <v>-0.004610612557683294</v>
       </c>
       <c r="J397">
-        <v>0.02447607861564227</v>
+        <v>0.02447646208579907</v>
       </c>
     </row>
     <row r="398" spans="1:10">
@@ -20224,7 +20143,7 @@
         <v>0.0117309228756987</v>
       </c>
       <c r="J398">
-        <v>0.0244764620857991</v>
+        <v>0.02446107227210579</v>
       </c>
     </row>
     <row r="399" spans="1:10">
@@ -20256,7 +20175,7 @@
         <v>0.009752291442678302</v>
       </c>
       <c r="J399">
-        <v>0.02446107227210581</v>
+        <v>0.01796044538054787</v>
       </c>
     </row>
     <row r="400" spans="1:10">
@@ -20288,7 +20207,7 @@
         <v>-0.007931370326280281</v>
       </c>
       <c r="J400">
-        <v>0.0179604453805479</v>
+        <v>0.01717075273293666</v>
       </c>
     </row>
     <row r="401" spans="1:10">
@@ -20320,7 +20239,7 @@
         <v>0.001399020913707409</v>
       </c>
       <c r="J401">
-        <v>0.01717075273293669</v>
+        <v>0.01684463838072308</v>
       </c>
     </row>
     <row r="402" spans="1:10">
@@ -20352,7 +20271,7 @@
         <v>0.01084102317787477</v>
       </c>
       <c r="J402">
-        <v>0.01684463838072311</v>
+        <v>0.01550669773373616</v>
       </c>
     </row>
     <row r="403" spans="1:10">
@@ -20384,7 +20303,7 @@
         <v>-0.001501126126267091</v>
       </c>
       <c r="J403">
-        <v>0.0155066977337362</v>
+        <v>0.01547627938250916</v>
       </c>
     </row>
     <row r="404" spans="1:10">
@@ -20416,7 +20335,7 @@
         <v>-0.004912044361020641</v>
       </c>
       <c r="J404">
-        <v>0.0154762793825092</v>
+        <v>0.01543977395949062</v>
       </c>
     </row>
     <row r="405" spans="1:10">
@@ -20448,7 +20367,7 @@
         <v>-0.05868899634867961</v>
       </c>
       <c r="J405">
-        <v>0.01543977395949066</v>
+        <v>0.01896643254468801</v>
       </c>
     </row>
     <row r="406" spans="1:10">
@@ -20480,7 +20399,7 @@
         <v>0.006578315360122507</v>
       </c>
       <c r="J406">
-        <v>0.01896643254468804</v>
+        <v>0.0189676481305849</v>
       </c>
     </row>
     <row r="407" spans="1:10">
@@ -20512,7 +20431,7 @@
         <v>0.005286004429237438</v>
       </c>
       <c r="J407">
-        <v>0.01896764813058493</v>
+        <v>0.01851450274985377</v>
       </c>
     </row>
     <row r="408" spans="1:10">
@@ -20544,7 +20463,7 @@
         <v>0.001399020913707409</v>
       </c>
       <c r="J408">
-        <v>0.0185145027498538</v>
+        <v>0.0185140894329141</v>
       </c>
     </row>
     <row r="409" spans="1:10">
@@ -20576,7 +20495,7 @@
         <v>0.0622233431801319</v>
       </c>
       <c r="J409">
-        <v>0.01851408943291413</v>
+        <v>0.02179133513527037</v>
       </c>
     </row>
     <row r="410" spans="1:10">
@@ -20608,7 +20527,7 @@
         <v>0.001798381941379397</v>
       </c>
       <c r="J410">
-        <v>0.0217913351352704</v>
+        <v>0.02178177297815928</v>
       </c>
     </row>
     <row r="411" spans="1:10">
@@ -20640,7 +20559,7 @@
         <v>-0.002503130218118477</v>
       </c>
       <c r="J411">
-        <v>0.02178177297815931</v>
+        <v>0.02047810007347266</v>
       </c>
     </row>
     <row r="412" spans="1:10">
@@ -20672,7 +20591,7 @@
         <v>-0.01857138558543534</v>
       </c>
       <c r="J412">
-        <v>0.02047810007347269</v>
+        <v>0.02070648938844664</v>
       </c>
     </row>
     <row r="413" spans="1:10">
@@ -20704,7 +20623,7 @@
         <v>-0.01308523954865548</v>
       </c>
       <c r="J413">
-        <v>0.02070648938844667</v>
+        <v>0.02083704034383423</v>
       </c>
     </row>
     <row r="414" spans="1:10">
@@ -20736,7 +20655,7 @@
         <v>0.009058844488346146</v>
       </c>
       <c r="J414">
-        <v>0.02083704034383427</v>
+        <v>0.02067392985296478</v>
       </c>
     </row>
     <row r="415" spans="1:10">
@@ -20768,7 +20687,7 @@
         <v>0.0006997551142732649</v>
       </c>
       <c r="J415">
-        <v>0.02067392985296481</v>
+        <v>0.01931463446937748</v>
       </c>
     </row>
     <row r="416" spans="1:10">
@@ -20800,7 +20719,7 @@
         <v>-0.003706861931326512</v>
       </c>
       <c r="J416">
-        <v>0.01931463446937752</v>
+        <v>0.01929884938887013</v>
       </c>
     </row>
     <row r="417" spans="1:10">
@@ -20832,7 +20751,7 @@
         <v>-0.002603385870114928</v>
       </c>
       <c r="J417">
-        <v>0.01929884938887017</v>
+        <v>0.01930068397645498</v>
       </c>
     </row>
     <row r="418" spans="1:10">
@@ -20864,7 +20783,7 @@
         <v>0.0005998200719675495</v>
       </c>
       <c r="J418">
-        <v>0.01930068397645501</v>
+        <v>0.01900031216553817</v>
       </c>
     </row>
     <row r="419" spans="1:10">
@@ -20896,7 +20815,7 @@
         <v>-0.004008021397538822</v>
       </c>
       <c r="J419">
-        <v>0.01900031216553821</v>
+        <v>0.0185205029592085</v>
       </c>
     </row>
     <row r="420" spans="1:10">
@@ -20928,7 +20847,7 @@
         <v>0.0004998750416509929</v>
       </c>
       <c r="J420">
-        <v>0.01852050295920853</v>
+        <v>0.01850653518512463</v>
       </c>
     </row>
     <row r="421" spans="1:10">
@@ -20960,7 +20879,7 @@
         <v>-0.004811556997222082</v>
       </c>
       <c r="J421">
-        <v>0.01850653518512467</v>
+        <v>0.01732760742898321</v>
       </c>
     </row>
     <row r="422" spans="1:10">
@@ -20992,7 +20911,7 @@
         <v>-0.001601281366973879</v>
       </c>
       <c r="J422">
-        <v>0.01732760742898325</v>
+        <v>0.01726780016646644</v>
       </c>
     </row>
     <row r="423" spans="1:10">
@@ -21024,7 +20943,7 @@
         <v>-0.02275698712261618</v>
       </c>
       <c r="J423">
-        <v>0.01726780016646648</v>
+        <v>0.01772004033828545</v>
       </c>
     </row>
     <row r="424" spans="1:10">
@@ -21056,7 +20975,7 @@
         <v>-0.002202423555200039</v>
       </c>
       <c r="J424">
-        <v>0.01772004033828549</v>
+        <v>0.01770932418266555</v>
       </c>
     </row>
     <row r="425" spans="1:10">
@@ -21088,7 +21007,7 @@
         <v>0.005982071677547469</v>
       </c>
       <c r="J425">
-        <v>0.01770932418266558</v>
+        <v>0.01776039718674017</v>
       </c>
     </row>
     <row r="426" spans="1:10">
@@ -21120,7 +21039,7 @@
         <v>0.004888034072775866</v>
       </c>
       <c r="J426">
-        <v>0.01776039718674021</v>
+        <v>0.0177056339978294</v>
       </c>
     </row>
     <row r="427" spans="1:10">
@@ -21152,7 +21071,7 @@
         <v>0.004290781417156246</v>
       </c>
       <c r="J427">
-        <v>0.01770563399782944</v>
+        <v>0.01771228372001183</v>
       </c>
     </row>
     <row r="428" spans="1:10">
@@ -21184,7 +21103,7 @@
         <v>-0.002102208091870198</v>
       </c>
       <c r="J428">
-        <v>0.01771228372001187</v>
+        <v>0.01756516641594843</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
enlarge the data range
</commit_message>
<xml_diff>
--- a/btc_data.xlsx
+++ b/btc_data.xlsx
@@ -408,7 +408,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L504"/>
+  <dimension ref="A1:L505"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -451,7 +451,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="1">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B2" s="2">
         <v>43025</v>
@@ -489,7 +489,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="B3" s="2">
         <v>43026</v>
@@ -527,7 +527,7 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="1">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B4" s="2">
         <v>43027</v>
@@ -565,7 +565,7 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="1">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B5" s="2">
         <v>43028</v>
@@ -603,7 +603,7 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="1">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B6" s="2">
         <v>43029</v>
@@ -641,7 +641,7 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="1">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B7" s="2">
         <v>43030</v>
@@ -679,7 +679,7 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="1">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B8" s="2">
         <v>43031</v>
@@ -717,7 +717,7 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="1">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B9" s="2">
         <v>43032</v>
@@ -755,7 +755,7 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="1">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="B10" s="2">
         <v>43033</v>
@@ -793,7 +793,7 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="1">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B11" s="2">
         <v>43034</v>
@@ -831,7 +831,7 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="1">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B12" s="2">
         <v>43035</v>
@@ -869,7 +869,7 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="1">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B13" s="2">
         <v>43036</v>
@@ -907,7 +907,7 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="1">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B14" s="2">
         <v>43037</v>
@@ -945,7 +945,7 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="1">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B15" s="2">
         <v>43038</v>
@@ -983,7 +983,7 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="1">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="B16" s="2">
         <v>43039</v>
@@ -1021,7 +1021,7 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="1">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="B17" s="2">
         <v>43040</v>
@@ -1059,7 +1059,7 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="1">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B18" s="2">
         <v>43041</v>
@@ -1097,7 +1097,7 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="1">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="B19" s="2">
         <v>43042</v>
@@ -1135,7 +1135,7 @@
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="1">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B20" s="2">
         <v>43043</v>
@@ -1173,7 +1173,7 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="1">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B21" s="2">
         <v>43044</v>
@@ -1211,7 +1211,7 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="1">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="B22" s="2">
         <v>43045</v>
@@ -1249,7 +1249,7 @@
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="1">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B23" s="2">
         <v>43046</v>
@@ -1287,7 +1287,7 @@
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="1">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="B24" s="2">
         <v>43047</v>
@@ -1325,7 +1325,7 @@
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="1">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B25" s="2">
         <v>43048</v>
@@ -1363,7 +1363,7 @@
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="1">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B26" s="2">
         <v>43049</v>
@@ -1401,7 +1401,7 @@
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="1">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B27" s="2">
         <v>43050</v>
@@ -1439,7 +1439,7 @@
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="1">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B28" s="2">
         <v>43051</v>
@@ -1477,7 +1477,7 @@
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="1">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B29" s="2">
         <v>43052</v>
@@ -1515,7 +1515,7 @@
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="1">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B30" s="2">
         <v>43053</v>
@@ -1553,7 +1553,7 @@
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="1">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B31" s="2">
         <v>43054</v>
@@ -1591,7 +1591,7 @@
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="1">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B32" s="2">
         <v>43055</v>
@@ -1629,7 +1629,7 @@
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="1">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B33" s="2">
         <v>43056</v>
@@ -1667,7 +1667,7 @@
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="1">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="B34" s="2">
         <v>43057</v>
@@ -1705,7 +1705,7 @@
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="1">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B35" s="2">
         <v>43058</v>
@@ -1743,7 +1743,7 @@
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="1">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="B36" s="2">
         <v>43059</v>
@@ -1781,7 +1781,7 @@
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="1">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B37" s="2">
         <v>43060</v>
@@ -1819,7 +1819,7 @@
     </row>
     <row r="38" spans="1:12">
       <c r="A38" s="1">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B38" s="2">
         <v>43061</v>
@@ -1857,7 +1857,7 @@
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="1">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="B39" s="2">
         <v>43062</v>
@@ -1895,7 +1895,7 @@
     </row>
     <row r="40" spans="1:12">
       <c r="A40" s="1">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="B40" s="2">
         <v>43063</v>
@@ -1933,7 +1933,7 @@
     </row>
     <row r="41" spans="1:12">
       <c r="A41" s="1">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B41" s="2">
         <v>43064</v>
@@ -1971,7 +1971,7 @@
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="1">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B42" s="2">
         <v>43065</v>
@@ -2009,7 +2009,7 @@
     </row>
     <row r="43" spans="1:12">
       <c r="A43" s="1">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="B43" s="2">
         <v>43066</v>
@@ -2047,7 +2047,7 @@
     </row>
     <row r="44" spans="1:12">
       <c r="A44" s="1">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B44" s="2">
         <v>43067</v>
@@ -2085,7 +2085,7 @@
     </row>
     <row r="45" spans="1:12">
       <c r="A45" s="1">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="B45" s="2">
         <v>43068</v>
@@ -2123,7 +2123,7 @@
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="1">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B46" s="2">
         <v>43069</v>
@@ -2161,7 +2161,7 @@
     </row>
     <row r="47" spans="1:12">
       <c r="A47" s="1">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B47" s="2">
         <v>43070</v>
@@ -2199,7 +2199,7 @@
     </row>
     <row r="48" spans="1:12">
       <c r="A48" s="1">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B48" s="2">
         <v>43071</v>
@@ -2237,7 +2237,7 @@
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="1">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B49" s="2">
         <v>43072</v>
@@ -2275,7 +2275,7 @@
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="1">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B50" s="2">
         <v>43073</v>
@@ -2313,7 +2313,7 @@
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="1">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B51" s="2">
         <v>43074</v>
@@ -2351,7 +2351,7 @@
     </row>
     <row r="52" spans="1:12">
       <c r="A52" s="1">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B52" s="2">
         <v>43075</v>
@@ -2389,7 +2389,7 @@
     </row>
     <row r="53" spans="1:12">
       <c r="A53" s="1">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B53" s="2">
         <v>43076</v>
@@ -2427,7 +2427,7 @@
     </row>
     <row r="54" spans="1:12">
       <c r="A54" s="1">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B54" s="2">
         <v>43077</v>
@@ -2465,7 +2465,7 @@
     </row>
     <row r="55" spans="1:12">
       <c r="A55" s="1">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B55" s="2">
         <v>43078</v>
@@ -2503,7 +2503,7 @@
     </row>
     <row r="56" spans="1:12">
       <c r="A56" s="1">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="B56" s="2">
         <v>43079</v>
@@ -2541,7 +2541,7 @@
     </row>
     <row r="57" spans="1:12">
       <c r="A57" s="1">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="B57" s="2">
         <v>43080</v>
@@ -2579,7 +2579,7 @@
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="1">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B58" s="2">
         <v>43081</v>
@@ -2617,7 +2617,7 @@
     </row>
     <row r="59" spans="1:12">
       <c r="A59" s="1">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="B59" s="2">
         <v>43082</v>
@@ -2655,7 +2655,7 @@
     </row>
     <row r="60" spans="1:12">
       <c r="A60" s="1">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B60" s="2">
         <v>43083</v>
@@ -2693,7 +2693,7 @@
     </row>
     <row r="61" spans="1:12">
       <c r="A61" s="1">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B61" s="2">
         <v>43084</v>
@@ -2731,7 +2731,7 @@
     </row>
     <row r="62" spans="1:12">
       <c r="A62" s="1">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B62" s="2">
         <v>43085</v>
@@ -2769,7 +2769,7 @@
     </row>
     <row r="63" spans="1:12">
       <c r="A63" s="1">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B63" s="2">
         <v>43086</v>
@@ -2807,7 +2807,7 @@
     </row>
     <row r="64" spans="1:12">
       <c r="A64" s="1">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B64" s="2">
         <v>43087</v>
@@ -2845,7 +2845,7 @@
     </row>
     <row r="65" spans="1:12">
       <c r="A65" s="1">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B65" s="2">
         <v>43088</v>
@@ -2883,7 +2883,7 @@
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="1">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="B66" s="2">
         <v>43089</v>
@@ -2921,7 +2921,7 @@
     </row>
     <row r="67" spans="1:12">
       <c r="A67" s="1">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B67" s="2">
         <v>43090</v>
@@ -2959,7 +2959,7 @@
     </row>
     <row r="68" spans="1:12">
       <c r="A68" s="1">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B68" s="2">
         <v>43091</v>
@@ -2997,7 +2997,7 @@
     </row>
     <row r="69" spans="1:12">
       <c r="A69" s="1">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B69" s="2">
         <v>43092</v>
@@ -3035,7 +3035,7 @@
     </row>
     <row r="70" spans="1:12">
       <c r="A70" s="1">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B70" s="2">
         <v>43093</v>
@@ -3073,7 +3073,7 @@
     </row>
     <row r="71" spans="1:12">
       <c r="A71" s="1">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B71" s="2">
         <v>43094</v>
@@ -3111,7 +3111,7 @@
     </row>
     <row r="72" spans="1:12">
       <c r="A72" s="1">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="B72" s="2">
         <v>43095</v>
@@ -3149,7 +3149,7 @@
     </row>
     <row r="73" spans="1:12">
       <c r="A73" s="1">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B73" s="2">
         <v>43096</v>
@@ -3187,7 +3187,7 @@
     </row>
     <row r="74" spans="1:12">
       <c r="A74" s="1">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B74" s="2">
         <v>43097</v>
@@ -3225,7 +3225,7 @@
     </row>
     <row r="75" spans="1:12">
       <c r="A75" s="1">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B75" s="2">
         <v>43098</v>
@@ -3263,7 +3263,7 @@
     </row>
     <row r="76" spans="1:12">
       <c r="A76" s="1">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B76" s="2">
         <v>43099</v>
@@ -3301,7 +3301,7 @@
     </row>
     <row r="77" spans="1:12">
       <c r="A77" s="1">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B77" s="2">
         <v>43100</v>
@@ -3339,7 +3339,7 @@
     </row>
     <row r="78" spans="1:12">
       <c r="A78" s="1">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B78" s="2">
         <v>43101</v>
@@ -3377,7 +3377,7 @@
     </row>
     <row r="79" spans="1:12">
       <c r="A79" s="1">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B79" s="2">
         <v>43102</v>
@@ -3415,7 +3415,7 @@
     </row>
     <row r="80" spans="1:12">
       <c r="A80" s="1">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B80" s="2">
         <v>43103</v>
@@ -3453,7 +3453,7 @@
     </row>
     <row r="81" spans="1:12">
       <c r="A81" s="1">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B81" s="2">
         <v>43104</v>
@@ -3491,7 +3491,7 @@
     </row>
     <row r="82" spans="1:12">
       <c r="A82" s="1">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B82" s="2">
         <v>43105</v>
@@ -3529,7 +3529,7 @@
     </row>
     <row r="83" spans="1:12">
       <c r="A83" s="1">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B83" s="2">
         <v>43106</v>
@@ -3567,7 +3567,7 @@
     </row>
     <row r="84" spans="1:12">
       <c r="A84" s="1">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B84" s="2">
         <v>43107</v>
@@ -3605,7 +3605,7 @@
     </row>
     <row r="85" spans="1:12">
       <c r="A85" s="1">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B85" s="2">
         <v>43108</v>
@@ -3643,7 +3643,7 @@
     </row>
     <row r="86" spans="1:12">
       <c r="A86" s="1">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B86" s="2">
         <v>43109</v>
@@ -3681,7 +3681,7 @@
     </row>
     <row r="87" spans="1:12">
       <c r="A87" s="1">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B87" s="2">
         <v>43110</v>
@@ -3719,7 +3719,7 @@
     </row>
     <row r="88" spans="1:12">
       <c r="A88" s="1">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B88" s="2">
         <v>43111</v>
@@ -3757,7 +3757,7 @@
     </row>
     <row r="89" spans="1:12">
       <c r="A89" s="1">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B89" s="2">
         <v>43112</v>
@@ -3795,7 +3795,7 @@
     </row>
     <row r="90" spans="1:12">
       <c r="A90" s="1">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B90" s="2">
         <v>43113</v>
@@ -3833,7 +3833,7 @@
     </row>
     <row r="91" spans="1:12">
       <c r="A91" s="1">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B91" s="2">
         <v>43114</v>
@@ -3871,7 +3871,7 @@
     </row>
     <row r="92" spans="1:12">
       <c r="A92" s="1">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B92" s="2">
         <v>43115</v>
@@ -3909,7 +3909,7 @@
     </row>
     <row r="93" spans="1:12">
       <c r="A93" s="1">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B93" s="2">
         <v>43116</v>
@@ -3947,7 +3947,7 @@
     </row>
     <row r="94" spans="1:12">
       <c r="A94" s="1">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B94" s="2">
         <v>43117</v>
@@ -3985,7 +3985,7 @@
     </row>
     <row r="95" spans="1:12">
       <c r="A95" s="1">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B95" s="2">
         <v>43118</v>
@@ -4023,7 +4023,7 @@
     </row>
     <row r="96" spans="1:12">
       <c r="A96" s="1">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B96" s="2">
         <v>43119</v>
@@ -4061,7 +4061,7 @@
     </row>
     <row r="97" spans="1:12">
       <c r="A97" s="1">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B97" s="2">
         <v>43120</v>
@@ -4099,7 +4099,7 @@
     </row>
     <row r="98" spans="1:12">
       <c r="A98" s="1">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B98" s="2">
         <v>43121</v>
@@ -4137,7 +4137,7 @@
     </row>
     <row r="99" spans="1:12">
       <c r="A99" s="1">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B99" s="2">
         <v>43122</v>
@@ -4175,7 +4175,7 @@
     </row>
     <row r="100" spans="1:12">
       <c r="A100" s="1">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B100" s="2">
         <v>43123</v>
@@ -4213,7 +4213,7 @@
     </row>
     <row r="101" spans="1:12">
       <c r="A101" s="1">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B101" s="2">
         <v>43124</v>
@@ -4251,7 +4251,7 @@
     </row>
     <row r="102" spans="1:12">
       <c r="A102" s="1">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B102" s="2">
         <v>43125</v>
@@ -4289,7 +4289,7 @@
     </row>
     <row r="103" spans="1:12">
       <c r="A103" s="1">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B103" s="2">
         <v>43126</v>
@@ -4327,7 +4327,7 @@
     </row>
     <row r="104" spans="1:12">
       <c r="A104" s="1">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B104" s="2">
         <v>43127</v>
@@ -4365,7 +4365,7 @@
     </row>
     <row r="105" spans="1:12">
       <c r="A105" s="1">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B105" s="2">
         <v>43128</v>
@@ -4403,7 +4403,7 @@
     </row>
     <row r="106" spans="1:12">
       <c r="A106" s="1">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B106" s="2">
         <v>43129</v>
@@ -4441,7 +4441,7 @@
     </row>
     <row r="107" spans="1:12">
       <c r="A107" s="1">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B107" s="2">
         <v>43130</v>
@@ -4479,7 +4479,7 @@
     </row>
     <row r="108" spans="1:12">
       <c r="A108" s="1">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B108" s="2">
         <v>43131</v>
@@ -4517,7 +4517,7 @@
     </row>
     <row r="109" spans="1:12">
       <c r="A109" s="1">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B109" s="2">
         <v>43132</v>
@@ -4555,7 +4555,7 @@
     </row>
     <row r="110" spans="1:12">
       <c r="A110" s="1">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B110" s="2">
         <v>43133</v>
@@ -4593,7 +4593,7 @@
     </row>
     <row r="111" spans="1:12">
       <c r="A111" s="1">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B111" s="2">
         <v>43134</v>
@@ -4631,7 +4631,7 @@
     </row>
     <row r="112" spans="1:12">
       <c r="A112" s="1">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B112" s="2">
         <v>43135</v>
@@ -4669,7 +4669,7 @@
     </row>
     <row r="113" spans="1:12">
       <c r="A113" s="1">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B113" s="2">
         <v>43136</v>
@@ -4707,7 +4707,7 @@
     </row>
     <row r="114" spans="1:12">
       <c r="A114" s="1">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B114" s="2">
         <v>43137</v>
@@ -4745,7 +4745,7 @@
     </row>
     <row r="115" spans="1:12">
       <c r="A115" s="1">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B115" s="2">
         <v>43138</v>
@@ -4783,7 +4783,7 @@
     </row>
     <row r="116" spans="1:12">
       <c r="A116" s="1">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B116" s="2">
         <v>43139</v>
@@ -4821,7 +4821,7 @@
     </row>
     <row r="117" spans="1:12">
       <c r="A117" s="1">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B117" s="2">
         <v>43140</v>
@@ -4859,7 +4859,7 @@
     </row>
     <row r="118" spans="1:12">
       <c r="A118" s="1">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B118" s="2">
         <v>43141</v>
@@ -4897,7 +4897,7 @@
     </row>
     <row r="119" spans="1:12">
       <c r="A119" s="1">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B119" s="2">
         <v>43142</v>
@@ -4935,7 +4935,7 @@
     </row>
     <row r="120" spans="1:12">
       <c r="A120" s="1">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B120" s="2">
         <v>43143</v>
@@ -4973,7 +4973,7 @@
     </row>
     <row r="121" spans="1:12">
       <c r="A121" s="1">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B121" s="2">
         <v>43144</v>
@@ -5011,7 +5011,7 @@
     </row>
     <row r="122" spans="1:12">
       <c r="A122" s="1">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B122" s="2">
         <v>43145</v>
@@ -5049,7 +5049,7 @@
     </row>
     <row r="123" spans="1:12">
       <c r="A123" s="1">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B123" s="2">
         <v>43146</v>
@@ -5087,7 +5087,7 @@
     </row>
     <row r="124" spans="1:12">
       <c r="A124" s="1">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B124" s="2">
         <v>43147</v>
@@ -5125,7 +5125,7 @@
     </row>
     <row r="125" spans="1:12">
       <c r="A125" s="1">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B125" s="2">
         <v>43148</v>
@@ -5163,7 +5163,7 @@
     </row>
     <row r="126" spans="1:12">
       <c r="A126" s="1">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B126" s="2">
         <v>43149</v>
@@ -5201,7 +5201,7 @@
     </row>
     <row r="127" spans="1:12">
       <c r="A127" s="1">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B127" s="2">
         <v>43150</v>
@@ -5239,7 +5239,7 @@
     </row>
     <row r="128" spans="1:12">
       <c r="A128" s="1">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B128" s="2">
         <v>43151</v>
@@ -5277,7 +5277,7 @@
     </row>
     <row r="129" spans="1:12">
       <c r="A129" s="1">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B129" s="2">
         <v>43152</v>
@@ -5315,7 +5315,7 @@
     </row>
     <row r="130" spans="1:12">
       <c r="A130" s="1">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B130" s="2">
         <v>43153</v>
@@ -5353,7 +5353,7 @@
     </row>
     <row r="131" spans="1:12">
       <c r="A131" s="1">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B131" s="2">
         <v>43154</v>
@@ -5391,7 +5391,7 @@
     </row>
     <row r="132" spans="1:12">
       <c r="A132" s="1">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B132" s="2">
         <v>43155</v>
@@ -5429,7 +5429,7 @@
     </row>
     <row r="133" spans="1:12">
       <c r="A133" s="1">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B133" s="2">
         <v>43156</v>
@@ -5467,7 +5467,7 @@
     </row>
     <row r="134" spans="1:12">
       <c r="A134" s="1">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B134" s="2">
         <v>43157</v>
@@ -5505,7 +5505,7 @@
     </row>
     <row r="135" spans="1:12">
       <c r="A135" s="1">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B135" s="2">
         <v>43158</v>
@@ -5543,7 +5543,7 @@
     </row>
     <row r="136" spans="1:12">
       <c r="A136" s="1">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B136" s="2">
         <v>43159</v>
@@ -5581,7 +5581,7 @@
     </row>
     <row r="137" spans="1:12">
       <c r="A137" s="1">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B137" s="2">
         <v>43160</v>
@@ -5619,7 +5619,7 @@
     </row>
     <row r="138" spans="1:12">
       <c r="A138" s="1">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B138" s="2">
         <v>43161</v>
@@ -5657,7 +5657,7 @@
     </row>
     <row r="139" spans="1:12">
       <c r="A139" s="1">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B139" s="2">
         <v>43162</v>
@@ -5695,7 +5695,7 @@
     </row>
     <row r="140" spans="1:12">
       <c r="A140" s="1">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B140" s="2">
         <v>43163</v>
@@ -5733,7 +5733,7 @@
     </row>
     <row r="141" spans="1:12">
       <c r="A141" s="1">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B141" s="2">
         <v>43164</v>
@@ -5771,7 +5771,7 @@
     </row>
     <row r="142" spans="1:12">
       <c r="A142" s="1">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B142" s="2">
         <v>43165</v>
@@ -5809,7 +5809,7 @@
     </row>
     <row r="143" spans="1:12">
       <c r="A143" s="1">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B143" s="2">
         <v>43166</v>
@@ -5847,7 +5847,7 @@
     </row>
     <row r="144" spans="1:12">
       <c r="A144" s="1">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B144" s="2">
         <v>43167</v>
@@ -5885,7 +5885,7 @@
     </row>
     <row r="145" spans="1:12">
       <c r="A145" s="1">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B145" s="2">
         <v>43168</v>
@@ -5923,7 +5923,7 @@
     </row>
     <row r="146" spans="1:12">
       <c r="A146" s="1">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B146" s="2">
         <v>43169</v>
@@ -5961,7 +5961,7 @@
     </row>
     <row r="147" spans="1:12">
       <c r="A147" s="1">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B147" s="2">
         <v>43170</v>
@@ -5999,7 +5999,7 @@
     </row>
     <row r="148" spans="1:12">
       <c r="A148" s="1">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B148" s="2">
         <v>43171</v>
@@ -6037,7 +6037,7 @@
     </row>
     <row r="149" spans="1:12">
       <c r="A149" s="1">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B149" s="2">
         <v>43172</v>
@@ -6075,7 +6075,7 @@
     </row>
     <row r="150" spans="1:12">
       <c r="A150" s="1">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B150" s="2">
         <v>43173</v>
@@ -6113,7 +6113,7 @@
     </row>
     <row r="151" spans="1:12">
       <c r="A151" s="1">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B151" s="2">
         <v>43174</v>
@@ -6151,7 +6151,7 @@
     </row>
     <row r="152" spans="1:12">
       <c r="A152" s="1">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B152" s="2">
         <v>43175</v>
@@ -6189,7 +6189,7 @@
     </row>
     <row r="153" spans="1:12">
       <c r="A153" s="1">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B153" s="2">
         <v>43176</v>
@@ -6227,7 +6227,7 @@
     </row>
     <row r="154" spans="1:12">
       <c r="A154" s="1">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B154" s="2">
         <v>43177</v>
@@ -6265,7 +6265,7 @@
     </row>
     <row r="155" spans="1:12">
       <c r="A155" s="1">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B155" s="2">
         <v>43178</v>
@@ -6303,7 +6303,7 @@
     </row>
     <row r="156" spans="1:12">
       <c r="A156" s="1">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B156" s="2">
         <v>43179</v>
@@ -6341,7 +6341,7 @@
     </row>
     <row r="157" spans="1:12">
       <c r="A157" s="1">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B157" s="2">
         <v>43180</v>
@@ -6379,7 +6379,7 @@
     </row>
     <row r="158" spans="1:12">
       <c r="A158" s="1">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B158" s="2">
         <v>43181</v>
@@ -6417,7 +6417,7 @@
     </row>
     <row r="159" spans="1:12">
       <c r="A159" s="1">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B159" s="2">
         <v>43182</v>
@@ -6455,7 +6455,7 @@
     </row>
     <row r="160" spans="1:12">
       <c r="A160" s="1">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B160" s="2">
         <v>43183</v>
@@ -6493,7 +6493,7 @@
     </row>
     <row r="161" spans="1:12">
       <c r="A161" s="1">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B161" s="2">
         <v>43184</v>
@@ -6531,7 +6531,7 @@
     </row>
     <row r="162" spans="1:12">
       <c r="A162" s="1">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B162" s="2">
         <v>43185</v>
@@ -6569,7 +6569,7 @@
     </row>
     <row r="163" spans="1:12">
       <c r="A163" s="1">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B163" s="2">
         <v>43186</v>
@@ -6607,7 +6607,7 @@
     </row>
     <row r="164" spans="1:12">
       <c r="A164" s="1">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B164" s="2">
         <v>43187</v>
@@ -6645,7 +6645,7 @@
     </row>
     <row r="165" spans="1:12">
       <c r="A165" s="1">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B165" s="2">
         <v>43188</v>
@@ -6683,7 +6683,7 @@
     </row>
     <row r="166" spans="1:12">
       <c r="A166" s="1">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B166" s="2">
         <v>43189</v>
@@ -6721,7 +6721,7 @@
     </row>
     <row r="167" spans="1:12">
       <c r="A167" s="1">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B167" s="2">
         <v>43190</v>
@@ -6759,7 +6759,7 @@
     </row>
     <row r="168" spans="1:12">
       <c r="A168" s="1">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B168" s="2">
         <v>43191</v>
@@ -6797,7 +6797,7 @@
     </row>
     <row r="169" spans="1:12">
       <c r="A169" s="1">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B169" s="2">
         <v>43192</v>
@@ -6835,7 +6835,7 @@
     </row>
     <row r="170" spans="1:12">
       <c r="A170" s="1">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B170" s="2">
         <v>43193</v>
@@ -6873,7 +6873,7 @@
     </row>
     <row r="171" spans="1:12">
       <c r="A171" s="1">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B171" s="2">
         <v>43194</v>
@@ -6911,7 +6911,7 @@
     </row>
     <row r="172" spans="1:12">
       <c r="A172" s="1">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B172" s="2">
         <v>43195</v>
@@ -6949,7 +6949,7 @@
     </row>
     <row r="173" spans="1:12">
       <c r="A173" s="1">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B173" s="2">
         <v>43196</v>
@@ -6987,7 +6987,7 @@
     </row>
     <row r="174" spans="1:12">
       <c r="A174" s="1">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B174" s="2">
         <v>43197</v>
@@ -7025,7 +7025,7 @@
     </row>
     <row r="175" spans="1:12">
       <c r="A175" s="1">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B175" s="2">
         <v>43198</v>
@@ -7063,7 +7063,7 @@
     </row>
     <row r="176" spans="1:12">
       <c r="A176" s="1">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B176" s="2">
         <v>43199</v>
@@ -7101,7 +7101,7 @@
     </row>
     <row r="177" spans="1:12">
       <c r="A177" s="1">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B177" s="2">
         <v>43200</v>
@@ -7139,7 +7139,7 @@
     </row>
     <row r="178" spans="1:12">
       <c r="A178" s="1">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B178" s="2">
         <v>43201</v>
@@ -7177,7 +7177,7 @@
     </row>
     <row r="179" spans="1:12">
       <c r="A179" s="1">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B179" s="2">
         <v>43202</v>
@@ -7215,7 +7215,7 @@
     </row>
     <row r="180" spans="1:12">
       <c r="A180" s="1">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B180" s="2">
         <v>43203</v>
@@ -7253,7 +7253,7 @@
     </row>
     <row r="181" spans="1:12">
       <c r="A181" s="1">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B181" s="2">
         <v>43204</v>
@@ -7291,7 +7291,7 @@
     </row>
     <row r="182" spans="1:12">
       <c r="A182" s="1">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B182" s="2">
         <v>43205</v>
@@ -7329,7 +7329,7 @@
     </row>
     <row r="183" spans="1:12">
       <c r="A183" s="1">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B183" s="2">
         <v>43206</v>
@@ -7367,7 +7367,7 @@
     </row>
     <row r="184" spans="1:12">
       <c r="A184" s="1">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B184" s="2">
         <v>43207</v>
@@ -7405,7 +7405,7 @@
     </row>
     <row r="185" spans="1:12">
       <c r="A185" s="1">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B185" s="2">
         <v>43208</v>
@@ -7443,7 +7443,7 @@
     </row>
     <row r="186" spans="1:12">
       <c r="A186" s="1">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B186" s="2">
         <v>43209</v>
@@ -7481,7 +7481,7 @@
     </row>
     <row r="187" spans="1:12">
       <c r="A187" s="1">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B187" s="2">
         <v>43210</v>
@@ -7519,7 +7519,7 @@
     </row>
     <row r="188" spans="1:12">
       <c r="A188" s="1">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B188" s="2">
         <v>43211</v>
@@ -7557,7 +7557,7 @@
     </row>
     <row r="189" spans="1:12">
       <c r="A189" s="1">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B189" s="2">
         <v>43212</v>
@@ -7595,7 +7595,7 @@
     </row>
     <row r="190" spans="1:12">
       <c r="A190" s="1">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B190" s="2">
         <v>43213</v>
@@ -7633,7 +7633,7 @@
     </row>
     <row r="191" spans="1:12">
       <c r="A191" s="1">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B191" s="2">
         <v>43214</v>
@@ -7671,7 +7671,7 @@
     </row>
     <row r="192" spans="1:12">
       <c r="A192" s="1">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B192" s="2">
         <v>43215</v>
@@ -7709,7 +7709,7 @@
     </row>
     <row r="193" spans="1:12">
       <c r="A193" s="1">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B193" s="2">
         <v>43216</v>
@@ -7747,7 +7747,7 @@
     </row>
     <row r="194" spans="1:12">
       <c r="A194" s="1">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B194" s="2">
         <v>43217</v>
@@ -7785,7 +7785,7 @@
     </row>
     <row r="195" spans="1:12">
       <c r="A195" s="1">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B195" s="2">
         <v>43218</v>
@@ -7823,7 +7823,7 @@
     </row>
     <row r="196" spans="1:12">
       <c r="A196" s="1">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B196" s="2">
         <v>43219</v>
@@ -7861,7 +7861,7 @@
     </row>
     <row r="197" spans="1:12">
       <c r="A197" s="1">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B197" s="2">
         <v>43220</v>
@@ -7899,7 +7899,7 @@
     </row>
     <row r="198" spans="1:12">
       <c r="A198" s="1">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B198" s="2">
         <v>43221</v>
@@ -7937,7 +7937,7 @@
     </row>
     <row r="199" spans="1:12">
       <c r="A199" s="1">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B199" s="2">
         <v>43222</v>
@@ -7975,7 +7975,7 @@
     </row>
     <row r="200" spans="1:12">
       <c r="A200" s="1">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B200" s="2">
         <v>43223</v>
@@ -8013,7 +8013,7 @@
     </row>
     <row r="201" spans="1:12">
       <c r="A201" s="1">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B201" s="2">
         <v>43224</v>
@@ -8051,7 +8051,7 @@
     </row>
     <row r="202" spans="1:12">
       <c r="A202" s="1">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B202" s="2">
         <v>43225</v>
@@ -8089,7 +8089,7 @@
     </row>
     <row r="203" spans="1:12">
       <c r="A203" s="1">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B203" s="2">
         <v>43226</v>
@@ -8127,7 +8127,7 @@
     </row>
     <row r="204" spans="1:12">
       <c r="A204" s="1">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B204" s="2">
         <v>43227</v>
@@ -8165,7 +8165,7 @@
     </row>
     <row r="205" spans="1:12">
       <c r="A205" s="1">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B205" s="2">
         <v>43228</v>
@@ -8203,7 +8203,7 @@
     </row>
     <row r="206" spans="1:12">
       <c r="A206" s="1">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B206" s="2">
         <v>43229</v>
@@ -8241,7 +8241,7 @@
     </row>
     <row r="207" spans="1:12">
       <c r="A207" s="1">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B207" s="2">
         <v>43230</v>
@@ -8279,7 +8279,7 @@
     </row>
     <row r="208" spans="1:12">
       <c r="A208" s="1">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B208" s="2">
         <v>43231</v>
@@ -8317,7 +8317,7 @@
     </row>
     <row r="209" spans="1:12">
       <c r="A209" s="1">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B209" s="2">
         <v>43232</v>
@@ -8355,7 +8355,7 @@
     </row>
     <row r="210" spans="1:12">
       <c r="A210" s="1">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B210" s="2">
         <v>43233</v>
@@ -8393,7 +8393,7 @@
     </row>
     <row r="211" spans="1:12">
       <c r="A211" s="1">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B211" s="2">
         <v>43234</v>
@@ -8431,7 +8431,7 @@
     </row>
     <row r="212" spans="1:12">
       <c r="A212" s="1">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B212" s="2">
         <v>43235</v>
@@ -8469,7 +8469,7 @@
     </row>
     <row r="213" spans="1:12">
       <c r="A213" s="1">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B213" s="2">
         <v>43236</v>
@@ -8507,7 +8507,7 @@
     </row>
     <row r="214" spans="1:12">
       <c r="A214" s="1">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B214" s="2">
         <v>43237</v>
@@ -8545,7 +8545,7 @@
     </row>
     <row r="215" spans="1:12">
       <c r="A215" s="1">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B215" s="2">
         <v>43238</v>
@@ -8583,7 +8583,7 @@
     </row>
     <row r="216" spans="1:12">
       <c r="A216" s="1">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B216" s="2">
         <v>43239</v>
@@ -8621,7 +8621,7 @@
     </row>
     <row r="217" spans="1:12">
       <c r="A217" s="1">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B217" s="2">
         <v>43240</v>
@@ -8659,7 +8659,7 @@
     </row>
     <row r="218" spans="1:12">
       <c r="A218" s="1">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B218" s="2">
         <v>43241</v>
@@ -8697,7 +8697,7 @@
     </row>
     <row r="219" spans="1:12">
       <c r="A219" s="1">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B219" s="2">
         <v>43242</v>
@@ -8735,7 +8735,7 @@
     </row>
     <row r="220" spans="1:12">
       <c r="A220" s="1">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B220" s="2">
         <v>43243</v>
@@ -8773,7 +8773,7 @@
     </row>
     <row r="221" spans="1:12">
       <c r="A221" s="1">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B221" s="2">
         <v>43244</v>
@@ -8811,7 +8811,7 @@
     </row>
     <row r="222" spans="1:12">
       <c r="A222" s="1">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B222" s="2">
         <v>43245</v>
@@ -8849,7 +8849,7 @@
     </row>
     <row r="223" spans="1:12">
       <c r="A223" s="1">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B223" s="2">
         <v>43246</v>
@@ -8887,7 +8887,7 @@
     </row>
     <row r="224" spans="1:12">
       <c r="A224" s="1">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B224" s="2">
         <v>43247</v>
@@ -8925,7 +8925,7 @@
     </row>
     <row r="225" spans="1:12">
       <c r="A225" s="1">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B225" s="2">
         <v>43248</v>
@@ -8963,7 +8963,7 @@
     </row>
     <row r="226" spans="1:12">
       <c r="A226" s="1">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B226" s="2">
         <v>43249</v>
@@ -9001,7 +9001,7 @@
     </row>
     <row r="227" spans="1:12">
       <c r="A227" s="1">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B227" s="2">
         <v>43250</v>
@@ -9039,7 +9039,7 @@
     </row>
     <row r="228" spans="1:12">
       <c r="A228" s="1">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B228" s="2">
         <v>43251</v>
@@ -9077,7 +9077,7 @@
     </row>
     <row r="229" spans="1:12">
       <c r="A229" s="1">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B229" s="2">
         <v>43252</v>
@@ -9115,7 +9115,7 @@
     </row>
     <row r="230" spans="1:12">
       <c r="A230" s="1">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B230" s="2">
         <v>43253</v>
@@ -9153,7 +9153,7 @@
     </row>
     <row r="231" spans="1:12">
       <c r="A231" s="1">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B231" s="2">
         <v>43254</v>
@@ -9191,7 +9191,7 @@
     </row>
     <row r="232" spans="1:12">
       <c r="A232" s="1">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B232" s="2">
         <v>43255</v>
@@ -9229,7 +9229,7 @@
     </row>
     <row r="233" spans="1:12">
       <c r="A233" s="1">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B233" s="2">
         <v>43256</v>
@@ -9267,7 +9267,7 @@
     </row>
     <row r="234" spans="1:12">
       <c r="A234" s="1">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B234" s="2">
         <v>43257</v>
@@ -9305,7 +9305,7 @@
     </row>
     <row r="235" spans="1:12">
       <c r="A235" s="1">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B235" s="2">
         <v>43258</v>
@@ -9343,7 +9343,7 @@
     </row>
     <row r="236" spans="1:12">
       <c r="A236" s="1">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B236" s="2">
         <v>43259</v>
@@ -9381,7 +9381,7 @@
     </row>
     <row r="237" spans="1:12">
       <c r="A237" s="1">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B237" s="2">
         <v>43260</v>
@@ -9419,7 +9419,7 @@
     </row>
     <row r="238" spans="1:12">
       <c r="A238" s="1">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B238" s="2">
         <v>43261</v>
@@ -9457,7 +9457,7 @@
     </row>
     <row r="239" spans="1:12">
       <c r="A239" s="1">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B239" s="2">
         <v>43262</v>
@@ -9495,7 +9495,7 @@
     </row>
     <row r="240" spans="1:12">
       <c r="A240" s="1">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B240" s="2">
         <v>43263</v>
@@ -9533,7 +9533,7 @@
     </row>
     <row r="241" spans="1:12">
       <c r="A241" s="1">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B241" s="2">
         <v>43264</v>
@@ -9571,7 +9571,7 @@
     </row>
     <row r="242" spans="1:12">
       <c r="A242" s="1">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B242" s="2">
         <v>43265</v>
@@ -9609,7 +9609,7 @@
     </row>
     <row r="243" spans="1:12">
       <c r="A243" s="1">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B243" s="2">
         <v>43266</v>
@@ -9647,7 +9647,7 @@
     </row>
     <row r="244" spans="1:12">
       <c r="A244" s="1">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B244" s="2">
         <v>43267</v>
@@ -9685,7 +9685,7 @@
     </row>
     <row r="245" spans="1:12">
       <c r="A245" s="1">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B245" s="2">
         <v>43268</v>
@@ -9723,7 +9723,7 @@
     </row>
     <row r="246" spans="1:12">
       <c r="A246" s="1">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B246" s="2">
         <v>43269</v>
@@ -9761,7 +9761,7 @@
     </row>
     <row r="247" spans="1:12">
       <c r="A247" s="1">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B247" s="2">
         <v>43270</v>
@@ -9799,7 +9799,7 @@
     </row>
     <row r="248" spans="1:12">
       <c r="A248" s="1">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B248" s="2">
         <v>43271</v>
@@ -9837,7 +9837,7 @@
     </row>
     <row r="249" spans="1:12">
       <c r="A249" s="1">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B249" s="2">
         <v>43272</v>
@@ -9875,7 +9875,7 @@
     </row>
     <row r="250" spans="1:12">
       <c r="A250" s="1">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B250" s="2">
         <v>43273</v>
@@ -9913,7 +9913,7 @@
     </row>
     <row r="251" spans="1:12">
       <c r="A251" s="1">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B251" s="2">
         <v>43274</v>
@@ -9951,7 +9951,7 @@
     </row>
     <row r="252" spans="1:12">
       <c r="A252" s="1">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B252" s="2">
         <v>43275</v>
@@ -9989,7 +9989,7 @@
     </row>
     <row r="253" spans="1:12">
       <c r="A253" s="1">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B253" s="2">
         <v>43276</v>
@@ -10027,7 +10027,7 @@
     </row>
     <row r="254" spans="1:12">
       <c r="A254" s="1">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B254" s="2">
         <v>43277</v>
@@ -10065,7 +10065,7 @@
     </row>
     <row r="255" spans="1:12">
       <c r="A255" s="1">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B255" s="2">
         <v>43278</v>
@@ -10103,7 +10103,7 @@
     </row>
     <row r="256" spans="1:12">
       <c r="A256" s="1">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B256" s="2">
         <v>43279</v>
@@ -10141,7 +10141,7 @@
     </row>
     <row r="257" spans="1:12">
       <c r="A257" s="1">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B257" s="2">
         <v>43280</v>
@@ -10179,7 +10179,7 @@
     </row>
     <row r="258" spans="1:12">
       <c r="A258" s="1">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B258" s="2">
         <v>43281</v>
@@ -10217,7 +10217,7 @@
     </row>
     <row r="259" spans="1:12">
       <c r="A259" s="1">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B259" s="2">
         <v>43282</v>
@@ -10255,7 +10255,7 @@
     </row>
     <row r="260" spans="1:12">
       <c r="A260" s="1">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B260" s="2">
         <v>43283</v>
@@ -10293,7 +10293,7 @@
     </row>
     <row r="261" spans="1:12">
       <c r="A261" s="1">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B261" s="2">
         <v>43284</v>
@@ -10331,7 +10331,7 @@
     </row>
     <row r="262" spans="1:12">
       <c r="A262" s="1">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B262" s="2">
         <v>43285</v>
@@ -10369,7 +10369,7 @@
     </row>
     <row r="263" spans="1:12">
       <c r="A263" s="1">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B263" s="2">
         <v>43286</v>
@@ -10407,7 +10407,7 @@
     </row>
     <row r="264" spans="1:12">
       <c r="A264" s="1">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B264" s="2">
         <v>43287</v>
@@ -10445,7 +10445,7 @@
     </row>
     <row r="265" spans="1:12">
       <c r="A265" s="1">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B265" s="2">
         <v>43288</v>
@@ -10483,7 +10483,7 @@
     </row>
     <row r="266" spans="1:12">
       <c r="A266" s="1">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B266" s="2">
         <v>43289</v>
@@ -10521,7 +10521,7 @@
     </row>
     <row r="267" spans="1:12">
       <c r="A267" s="1">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B267" s="2">
         <v>43290</v>
@@ -10559,7 +10559,7 @@
     </row>
     <row r="268" spans="1:12">
       <c r="A268" s="1">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B268" s="2">
         <v>43291</v>
@@ -10597,7 +10597,7 @@
     </row>
     <row r="269" spans="1:12">
       <c r="A269" s="1">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B269" s="2">
         <v>43292</v>
@@ -10635,7 +10635,7 @@
     </row>
     <row r="270" spans="1:12">
       <c r="A270" s="1">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B270" s="2">
         <v>43293</v>
@@ -10673,7 +10673,7 @@
     </row>
     <row r="271" spans="1:12">
       <c r="A271" s="1">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B271" s="2">
         <v>43294</v>
@@ -10711,7 +10711,7 @@
     </row>
     <row r="272" spans="1:12">
       <c r="A272" s="1">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B272" s="2">
         <v>43295</v>
@@ -10749,7 +10749,7 @@
     </row>
     <row r="273" spans="1:12">
       <c r="A273" s="1">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B273" s="2">
         <v>43296</v>
@@ -10787,7 +10787,7 @@
     </row>
     <row r="274" spans="1:12">
       <c r="A274" s="1">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B274" s="2">
         <v>43297</v>
@@ -10825,7 +10825,7 @@
     </row>
     <row r="275" spans="1:12">
       <c r="A275" s="1">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B275" s="2">
         <v>43298</v>
@@ -10863,7 +10863,7 @@
     </row>
     <row r="276" spans="1:12">
       <c r="A276" s="1">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B276" s="2">
         <v>43299</v>
@@ -10901,7 +10901,7 @@
     </row>
     <row r="277" spans="1:12">
       <c r="A277" s="1">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B277" s="2">
         <v>43300</v>
@@ -10939,7 +10939,7 @@
     </row>
     <row r="278" spans="1:12">
       <c r="A278" s="1">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B278" s="2">
         <v>43301</v>
@@ -10977,7 +10977,7 @@
     </row>
     <row r="279" spans="1:12">
       <c r="A279" s="1">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B279" s="2">
         <v>43302</v>
@@ -11015,7 +11015,7 @@
     </row>
     <row r="280" spans="1:12">
       <c r="A280" s="1">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B280" s="2">
         <v>43303</v>
@@ -11053,7 +11053,7 @@
     </row>
     <row r="281" spans="1:12">
       <c r="A281" s="1">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B281" s="2">
         <v>43304</v>
@@ -11091,7 +11091,7 @@
     </row>
     <row r="282" spans="1:12">
       <c r="A282" s="1">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B282" s="2">
         <v>43305</v>
@@ -11129,7 +11129,7 @@
     </row>
     <row r="283" spans="1:12">
       <c r="A283" s="1">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B283" s="2">
         <v>43306</v>
@@ -11167,7 +11167,7 @@
     </row>
     <row r="284" spans="1:12">
       <c r="A284" s="1">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B284" s="2">
         <v>43307</v>
@@ -11205,7 +11205,7 @@
     </row>
     <row r="285" spans="1:12">
       <c r="A285" s="1">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B285" s="2">
         <v>43308</v>
@@ -11243,7 +11243,7 @@
     </row>
     <row r="286" spans="1:12">
       <c r="A286" s="1">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B286" s="2">
         <v>43309</v>
@@ -11281,7 +11281,7 @@
     </row>
     <row r="287" spans="1:12">
       <c r="A287" s="1">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B287" s="2">
         <v>43310</v>
@@ -11319,7 +11319,7 @@
     </row>
     <row r="288" spans="1:12">
       <c r="A288" s="1">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B288" s="2">
         <v>43311</v>
@@ -11357,7 +11357,7 @@
     </row>
     <row r="289" spans="1:12">
       <c r="A289" s="1">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B289" s="2">
         <v>43312</v>
@@ -11395,7 +11395,7 @@
     </row>
     <row r="290" spans="1:12">
       <c r="A290" s="1">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B290" s="2">
         <v>43313</v>
@@ -11433,7 +11433,7 @@
     </row>
     <row r="291" spans="1:12">
       <c r="A291" s="1">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B291" s="2">
         <v>43314</v>
@@ -11471,7 +11471,7 @@
     </row>
     <row r="292" spans="1:12">
       <c r="A292" s="1">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B292" s="2">
         <v>43315</v>
@@ -11509,7 +11509,7 @@
     </row>
     <row r="293" spans="1:12">
       <c r="A293" s="1">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B293" s="2">
         <v>43316</v>
@@ -11547,7 +11547,7 @@
     </row>
     <row r="294" spans="1:12">
       <c r="A294" s="1">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B294" s="2">
         <v>43317</v>
@@ -11585,7 +11585,7 @@
     </row>
     <row r="295" spans="1:12">
       <c r="A295" s="1">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B295" s="2">
         <v>43318</v>
@@ -11623,7 +11623,7 @@
     </row>
     <row r="296" spans="1:12">
       <c r="A296" s="1">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B296" s="2">
         <v>43319</v>
@@ -11661,7 +11661,7 @@
     </row>
     <row r="297" spans="1:12">
       <c r="A297" s="1">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B297" s="2">
         <v>43320</v>
@@ -11699,7 +11699,7 @@
     </row>
     <row r="298" spans="1:12">
       <c r="A298" s="1">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B298" s="2">
         <v>43321</v>
@@ -11737,7 +11737,7 @@
     </row>
     <row r="299" spans="1:12">
       <c r="A299" s="1">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B299" s="2">
         <v>43322</v>
@@ -11775,7 +11775,7 @@
     </row>
     <row r="300" spans="1:12">
       <c r="A300" s="1">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B300" s="2">
         <v>43323</v>
@@ -11813,7 +11813,7 @@
     </row>
     <row r="301" spans="1:12">
       <c r="A301" s="1">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B301" s="2">
         <v>43324</v>
@@ -11851,7 +11851,7 @@
     </row>
     <row r="302" spans="1:12">
       <c r="A302" s="1">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B302" s="2">
         <v>43325</v>
@@ -11889,7 +11889,7 @@
     </row>
     <row r="303" spans="1:12">
       <c r="A303" s="1">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B303" s="2">
         <v>43326</v>
@@ -11927,7 +11927,7 @@
     </row>
     <row r="304" spans="1:12">
       <c r="A304" s="1">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B304" s="2">
         <v>43327</v>
@@ -11965,7 +11965,7 @@
     </row>
     <row r="305" spans="1:12">
       <c r="A305" s="1">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B305" s="2">
         <v>43328</v>
@@ -12003,7 +12003,7 @@
     </row>
     <row r="306" spans="1:12">
       <c r="A306" s="1">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B306" s="2">
         <v>43329</v>
@@ -12041,7 +12041,7 @@
     </row>
     <row r="307" spans="1:12">
       <c r="A307" s="1">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B307" s="2">
         <v>43330</v>
@@ -12079,7 +12079,7 @@
     </row>
     <row r="308" spans="1:12">
       <c r="A308" s="1">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B308" s="2">
         <v>43331</v>
@@ -12117,7 +12117,7 @@
     </row>
     <row r="309" spans="1:12">
       <c r="A309" s="1">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B309" s="2">
         <v>43332</v>
@@ -12155,7 +12155,7 @@
     </row>
     <row r="310" spans="1:12">
       <c r="A310" s="1">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B310" s="2">
         <v>43333</v>
@@ -12193,7 +12193,7 @@
     </row>
     <row r="311" spans="1:12">
       <c r="A311" s="1">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B311" s="2">
         <v>43334</v>
@@ -12231,7 +12231,7 @@
     </row>
     <row r="312" spans="1:12">
       <c r="A312" s="1">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B312" s="2">
         <v>43335</v>
@@ -12269,7 +12269,7 @@
     </row>
     <row r="313" spans="1:12">
       <c r="A313" s="1">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B313" s="2">
         <v>43336</v>
@@ -12307,7 +12307,7 @@
     </row>
     <row r="314" spans="1:12">
       <c r="A314" s="1">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B314" s="2">
         <v>43337</v>
@@ -12345,7 +12345,7 @@
     </row>
     <row r="315" spans="1:12">
       <c r="A315" s="1">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B315" s="2">
         <v>43338</v>
@@ -12383,7 +12383,7 @@
     </row>
     <row r="316" spans="1:12">
       <c r="A316" s="1">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B316" s="2">
         <v>43339</v>
@@ -12421,7 +12421,7 @@
     </row>
     <row r="317" spans="1:12">
       <c r="A317" s="1">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B317" s="2">
         <v>43340</v>
@@ -12459,7 +12459,7 @@
     </row>
     <row r="318" spans="1:12">
       <c r="A318" s="1">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B318" s="2">
         <v>43341</v>
@@ -12497,7 +12497,7 @@
     </row>
     <row r="319" spans="1:12">
       <c r="A319" s="1">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B319" s="2">
         <v>43342</v>
@@ -12535,7 +12535,7 @@
     </row>
     <row r="320" spans="1:12">
       <c r="A320" s="1">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B320" s="2">
         <v>43343</v>
@@ -12573,7 +12573,7 @@
     </row>
     <row r="321" spans="1:12">
       <c r="A321" s="1">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B321" s="2">
         <v>43344</v>
@@ -12611,7 +12611,7 @@
     </row>
     <row r="322" spans="1:12">
       <c r="A322" s="1">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B322" s="2">
         <v>43345</v>
@@ -12649,7 +12649,7 @@
     </row>
     <row r="323" spans="1:12">
       <c r="A323" s="1">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B323" s="2">
         <v>43346</v>
@@ -12687,7 +12687,7 @@
     </row>
     <row r="324" spans="1:12">
       <c r="A324" s="1">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B324" s="2">
         <v>43347</v>
@@ -12725,7 +12725,7 @@
     </row>
     <row r="325" spans="1:12">
       <c r="A325" s="1">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B325" s="2">
         <v>43348</v>
@@ -12763,7 +12763,7 @@
     </row>
     <row r="326" spans="1:12">
       <c r="A326" s="1">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B326" s="2">
         <v>43349</v>
@@ -12801,7 +12801,7 @@
     </row>
     <row r="327" spans="1:12">
       <c r="A327" s="1">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B327" s="2">
         <v>43350</v>
@@ -12839,7 +12839,7 @@
     </row>
     <row r="328" spans="1:12">
       <c r="A328" s="1">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B328" s="2">
         <v>43351</v>
@@ -12877,7 +12877,7 @@
     </row>
     <row r="329" spans="1:12">
       <c r="A329" s="1">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B329" s="2">
         <v>43352</v>
@@ -12915,7 +12915,7 @@
     </row>
     <row r="330" spans="1:12">
       <c r="A330" s="1">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B330" s="2">
         <v>43353</v>
@@ -12953,7 +12953,7 @@
     </row>
     <row r="331" spans="1:12">
       <c r="A331" s="1">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B331" s="2">
         <v>43354</v>
@@ -12991,7 +12991,7 @@
     </row>
     <row r="332" spans="1:12">
       <c r="A332" s="1">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B332" s="2">
         <v>43355</v>
@@ -13029,7 +13029,7 @@
     </row>
     <row r="333" spans="1:12">
       <c r="A333" s="1">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B333" s="2">
         <v>43356</v>
@@ -13067,7 +13067,7 @@
     </row>
     <row r="334" spans="1:12">
       <c r="A334" s="1">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B334" s="2">
         <v>43357</v>
@@ -13105,7 +13105,7 @@
     </row>
     <row r="335" spans="1:12">
       <c r="A335" s="1">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B335" s="2">
         <v>43358</v>
@@ -13143,7 +13143,7 @@
     </row>
     <row r="336" spans="1:12">
       <c r="A336" s="1">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B336" s="2">
         <v>43359</v>
@@ -13181,7 +13181,7 @@
     </row>
     <row r="337" spans="1:12">
       <c r="A337" s="1">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B337" s="2">
         <v>43360</v>
@@ -13219,7 +13219,7 @@
     </row>
     <row r="338" spans="1:12">
       <c r="A338" s="1">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B338" s="2">
         <v>43361</v>
@@ -13257,7 +13257,7 @@
     </row>
     <row r="339" spans="1:12">
       <c r="A339" s="1">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B339" s="2">
         <v>43362</v>
@@ -13295,7 +13295,7 @@
     </row>
     <row r="340" spans="1:12">
       <c r="A340" s="1">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B340" s="2">
         <v>43363</v>
@@ -13333,7 +13333,7 @@
     </row>
     <row r="341" spans="1:12">
       <c r="A341" s="1">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B341" s="2">
         <v>43364</v>
@@ -13371,7 +13371,7 @@
     </row>
     <row r="342" spans="1:12">
       <c r="A342" s="1">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B342" s="2">
         <v>43365</v>
@@ -13409,7 +13409,7 @@
     </row>
     <row r="343" spans="1:12">
       <c r="A343" s="1">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B343" s="2">
         <v>43366</v>
@@ -13447,7 +13447,7 @@
     </row>
     <row r="344" spans="1:12">
       <c r="A344" s="1">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B344" s="2">
         <v>43367</v>
@@ -13485,7 +13485,7 @@
     </row>
     <row r="345" spans="1:12">
       <c r="A345" s="1">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B345" s="2">
         <v>43368</v>
@@ -13523,7 +13523,7 @@
     </row>
     <row r="346" spans="1:12">
       <c r="A346" s="1">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B346" s="2">
         <v>43369</v>
@@ -13561,7 +13561,7 @@
     </row>
     <row r="347" spans="1:12">
       <c r="A347" s="1">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B347" s="2">
         <v>43370</v>
@@ -13599,7 +13599,7 @@
     </row>
     <row r="348" spans="1:12">
       <c r="A348" s="1">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B348" s="2">
         <v>43371</v>
@@ -13637,7 +13637,7 @@
     </row>
     <row r="349" spans="1:12">
       <c r="A349" s="1">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B349" s="2">
         <v>43372</v>
@@ -13675,7 +13675,7 @@
     </row>
     <row r="350" spans="1:12">
       <c r="A350" s="1">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B350" s="2">
         <v>43373</v>
@@ -13713,7 +13713,7 @@
     </row>
     <row r="351" spans="1:12">
       <c r="A351" s="1">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B351" s="2">
         <v>43374</v>
@@ -13751,7 +13751,7 @@
     </row>
     <row r="352" spans="1:12">
       <c r="A352" s="1">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B352" s="2">
         <v>43375</v>
@@ -13789,7 +13789,7 @@
     </row>
     <row r="353" spans="1:12">
       <c r="A353" s="1">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B353" s="2">
         <v>43376</v>
@@ -13827,7 +13827,7 @@
     </row>
     <row r="354" spans="1:12">
       <c r="A354" s="1">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B354" s="2">
         <v>43377</v>
@@ -13865,7 +13865,7 @@
     </row>
     <row r="355" spans="1:12">
       <c r="A355" s="1">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B355" s="2">
         <v>43378</v>
@@ -13903,7 +13903,7 @@
     </row>
     <row r="356" spans="1:12">
       <c r="A356" s="1">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B356" s="2">
         <v>43379</v>
@@ -13941,7 +13941,7 @@
     </row>
     <row r="357" spans="1:12">
       <c r="A357" s="1">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B357" s="2">
         <v>43380</v>
@@ -13979,7 +13979,7 @@
     </row>
     <row r="358" spans="1:12">
       <c r="A358" s="1">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B358" s="2">
         <v>43381</v>
@@ -14017,7 +14017,7 @@
     </row>
     <row r="359" spans="1:12">
       <c r="A359" s="1">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B359" s="2">
         <v>43382</v>
@@ -14055,7 +14055,7 @@
     </row>
     <row r="360" spans="1:12">
       <c r="A360" s="1">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B360" s="2">
         <v>43383</v>
@@ -14093,7 +14093,7 @@
     </row>
     <row r="361" spans="1:12">
       <c r="A361" s="1">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B361" s="2">
         <v>43384</v>
@@ -14131,7 +14131,7 @@
     </row>
     <row r="362" spans="1:12">
       <c r="A362" s="1">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B362" s="2">
         <v>43385</v>
@@ -14169,7 +14169,7 @@
     </row>
     <row r="363" spans="1:12">
       <c r="A363" s="1">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B363" s="2">
         <v>43386</v>
@@ -14207,7 +14207,7 @@
     </row>
     <row r="364" spans="1:12">
       <c r="A364" s="1">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B364" s="2">
         <v>43387</v>
@@ -14245,7 +14245,7 @@
     </row>
     <row r="365" spans="1:12">
       <c r="A365" s="1">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B365" s="2">
         <v>43388</v>
@@ -14283,7 +14283,7 @@
     </row>
     <row r="366" spans="1:12">
       <c r="A366" s="1">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B366" s="2">
         <v>43389</v>
@@ -14321,7 +14321,7 @@
     </row>
     <row r="367" spans="1:12">
       <c r="A367" s="1">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B367" s="2">
         <v>43390</v>
@@ -14359,7 +14359,7 @@
     </row>
     <row r="368" spans="1:12">
       <c r="A368" s="1">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B368" s="2">
         <v>43391</v>
@@ -14397,7 +14397,7 @@
     </row>
     <row r="369" spans="1:12">
       <c r="A369" s="1">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B369" s="2">
         <v>43392</v>
@@ -14435,7 +14435,7 @@
     </row>
     <row r="370" spans="1:12">
       <c r="A370" s="1">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B370" s="2">
         <v>43393</v>
@@ -14473,7 +14473,7 @@
     </row>
     <row r="371" spans="1:12">
       <c r="A371" s="1">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B371" s="2">
         <v>43394</v>
@@ -14511,7 +14511,7 @@
     </row>
     <row r="372" spans="1:12">
       <c r="A372" s="1">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B372" s="2">
         <v>43395</v>
@@ -14549,7 +14549,7 @@
     </row>
     <row r="373" spans="1:12">
       <c r="A373" s="1">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B373" s="2">
         <v>43396</v>
@@ -14587,7 +14587,7 @@
     </row>
     <row r="374" spans="1:12">
       <c r="A374" s="1">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B374" s="2">
         <v>43397</v>
@@ -14625,7 +14625,7 @@
     </row>
     <row r="375" spans="1:12">
       <c r="A375" s="1">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B375" s="2">
         <v>43398</v>
@@ -14663,7 +14663,7 @@
     </row>
     <row r="376" spans="1:12">
       <c r="A376" s="1">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B376" s="2">
         <v>43399</v>
@@ -14701,7 +14701,7 @@
     </row>
     <row r="377" spans="1:12">
       <c r="A377" s="1">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B377" s="2">
         <v>43400</v>
@@ -14739,7 +14739,7 @@
     </row>
     <row r="378" spans="1:12">
       <c r="A378" s="1">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B378" s="2">
         <v>43401</v>
@@ -14777,7 +14777,7 @@
     </row>
     <row r="379" spans="1:12">
       <c r="A379" s="1">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B379" s="2">
         <v>43402</v>
@@ -14815,7 +14815,7 @@
     </row>
     <row r="380" spans="1:12">
       <c r="A380" s="1">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B380" s="2">
         <v>43403</v>
@@ -14853,7 +14853,7 @@
     </row>
     <row r="381" spans="1:12">
       <c r="A381" s="1">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B381" s="2">
         <v>43404</v>
@@ -14891,7 +14891,7 @@
     </row>
     <row r="382" spans="1:12">
       <c r="A382" s="1">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B382" s="2">
         <v>43405</v>
@@ -14929,7 +14929,7 @@
     </row>
     <row r="383" spans="1:12">
       <c r="A383" s="1">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B383" s="2">
         <v>43406</v>
@@ -14967,7 +14967,7 @@
     </row>
     <row r="384" spans="1:12">
       <c r="A384" s="1">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B384" s="2">
         <v>43407</v>
@@ -15005,7 +15005,7 @@
     </row>
     <row r="385" spans="1:12">
       <c r="A385" s="1">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B385" s="2">
         <v>43408</v>
@@ -15043,7 +15043,7 @@
     </row>
     <row r="386" spans="1:12">
       <c r="A386" s="1">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B386" s="2">
         <v>43409</v>
@@ -15081,7 +15081,7 @@
     </row>
     <row r="387" spans="1:12">
       <c r="A387" s="1">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B387" s="2">
         <v>43410</v>
@@ -15119,7 +15119,7 @@
     </row>
     <row r="388" spans="1:12">
       <c r="A388" s="1">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B388" s="2">
         <v>43411</v>
@@ -15157,7 +15157,7 @@
     </row>
     <row r="389" spans="1:12">
       <c r="A389" s="1">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B389" s="2">
         <v>43412</v>
@@ -15195,7 +15195,7 @@
     </row>
     <row r="390" spans="1:12">
       <c r="A390" s="1">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B390" s="2">
         <v>43413</v>
@@ -15233,7 +15233,7 @@
     </row>
     <row r="391" spans="1:12">
       <c r="A391" s="1">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B391" s="2">
         <v>43414</v>
@@ -15271,7 +15271,7 @@
     </row>
     <row r="392" spans="1:12">
       <c r="A392" s="1">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B392" s="2">
         <v>43415</v>
@@ -15309,7 +15309,7 @@
     </row>
     <row r="393" spans="1:12">
       <c r="A393" s="1">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B393" s="2">
         <v>43416</v>
@@ -15347,7 +15347,7 @@
     </row>
     <row r="394" spans="1:12">
       <c r="A394" s="1">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B394" s="2">
         <v>43417</v>
@@ -15385,7 +15385,7 @@
     </row>
     <row r="395" spans="1:12">
       <c r="A395" s="1">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B395" s="2">
         <v>43418</v>
@@ -15423,7 +15423,7 @@
     </row>
     <row r="396" spans="1:12">
       <c r="A396" s="1">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B396" s="2">
         <v>43419</v>
@@ -15461,7 +15461,7 @@
     </row>
     <row r="397" spans="1:12">
       <c r="A397" s="1">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B397" s="2">
         <v>43420</v>
@@ -15499,7 +15499,7 @@
     </row>
     <row r="398" spans="1:12">
       <c r="A398" s="1">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B398" s="2">
         <v>43421</v>
@@ -15537,7 +15537,7 @@
     </row>
     <row r="399" spans="1:12">
       <c r="A399" s="1">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B399" s="2">
         <v>43422</v>
@@ -15575,7 +15575,7 @@
     </row>
     <row r="400" spans="1:12">
       <c r="A400" s="1">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B400" s="2">
         <v>43423</v>
@@ -15613,7 +15613,7 @@
     </row>
     <row r="401" spans="1:12">
       <c r="A401" s="1">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B401" s="2">
         <v>43424</v>
@@ -15651,7 +15651,7 @@
     </row>
     <row r="402" spans="1:12">
       <c r="A402" s="1">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B402" s="2">
         <v>43425</v>
@@ -15689,7 +15689,7 @@
     </row>
     <row r="403" spans="1:12">
       <c r="A403" s="1">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B403" s="2">
         <v>43426</v>
@@ -15727,7 +15727,7 @@
     </row>
     <row r="404" spans="1:12">
       <c r="A404" s="1">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B404" s="2">
         <v>43427</v>
@@ -15765,7 +15765,7 @@
     </row>
     <row r="405" spans="1:12">
       <c r="A405" s="1">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B405" s="2">
         <v>43428</v>
@@ -15803,7 +15803,7 @@
     </row>
     <row r="406" spans="1:12">
       <c r="A406" s="1">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B406" s="2">
         <v>43429</v>
@@ -15841,7 +15841,7 @@
     </row>
     <row r="407" spans="1:12">
       <c r="A407" s="1">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B407" s="2">
         <v>43430</v>
@@ -15879,7 +15879,7 @@
     </row>
     <row r="408" spans="1:12">
       <c r="A408" s="1">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B408" s="2">
         <v>43431</v>
@@ -15917,7 +15917,7 @@
     </row>
     <row r="409" spans="1:12">
       <c r="A409" s="1">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B409" s="2">
         <v>43432</v>
@@ -15955,7 +15955,7 @@
     </row>
     <row r="410" spans="1:12">
       <c r="A410" s="1">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B410" s="2">
         <v>43433</v>
@@ -15993,7 +15993,7 @@
     </row>
     <row r="411" spans="1:12">
       <c r="A411" s="1">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B411" s="2">
         <v>43434</v>
@@ -16031,7 +16031,7 @@
     </row>
     <row r="412" spans="1:12">
       <c r="A412" s="1">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B412" s="2">
         <v>43435</v>
@@ -16069,7 +16069,7 @@
     </row>
     <row r="413" spans="1:12">
       <c r="A413" s="1">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B413" s="2">
         <v>43436</v>
@@ -16107,7 +16107,7 @@
     </row>
     <row r="414" spans="1:12">
       <c r="A414" s="1">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B414" s="2">
         <v>43437</v>
@@ -16145,7 +16145,7 @@
     </row>
     <row r="415" spans="1:12">
       <c r="A415" s="1">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B415" s="2">
         <v>43438</v>
@@ -16183,7 +16183,7 @@
     </row>
     <row r="416" spans="1:12">
       <c r="A416" s="1">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B416" s="2">
         <v>43439</v>
@@ -16221,7 +16221,7 @@
     </row>
     <row r="417" spans="1:12">
       <c r="A417" s="1">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B417" s="2">
         <v>43440</v>
@@ -16259,7 +16259,7 @@
     </row>
     <row r="418" spans="1:12">
       <c r="A418" s="1">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B418" s="2">
         <v>43441</v>
@@ -16297,7 +16297,7 @@
     </row>
     <row r="419" spans="1:12">
       <c r="A419" s="1">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B419" s="2">
         <v>43442</v>
@@ -16335,7 +16335,7 @@
     </row>
     <row r="420" spans="1:12">
       <c r="A420" s="1">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B420" s="2">
         <v>43443</v>
@@ -16373,7 +16373,7 @@
     </row>
     <row r="421" spans="1:12">
       <c r="A421" s="1">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B421" s="2">
         <v>43444</v>
@@ -16411,7 +16411,7 @@
     </row>
     <row r="422" spans="1:12">
       <c r="A422" s="1">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B422" s="2">
         <v>43445</v>
@@ -16449,7 +16449,7 @@
     </row>
     <row r="423" spans="1:12">
       <c r="A423" s="1">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B423" s="2">
         <v>43446</v>
@@ -16487,7 +16487,7 @@
     </row>
     <row r="424" spans="1:12">
       <c r="A424" s="1">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B424" s="2">
         <v>43447</v>
@@ -16525,7 +16525,7 @@
     </row>
     <row r="425" spans="1:12">
       <c r="A425" s="1">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B425" s="2">
         <v>43448</v>
@@ -16563,7 +16563,7 @@
     </row>
     <row r="426" spans="1:12">
       <c r="A426" s="1">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B426" s="2">
         <v>43449</v>
@@ -16601,7 +16601,7 @@
     </row>
     <row r="427" spans="1:12">
       <c r="A427" s="1">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B427" s="2">
         <v>43450</v>
@@ -16639,7 +16639,7 @@
     </row>
     <row r="428" spans="1:12">
       <c r="A428" s="1">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B428" s="2">
         <v>43451</v>
@@ -16677,7 +16677,7 @@
     </row>
     <row r="429" spans="1:12">
       <c r="A429" s="1">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B429" s="2">
         <v>43452</v>
@@ -16715,7 +16715,7 @@
     </row>
     <row r="430" spans="1:12">
       <c r="A430" s="1">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B430" s="2">
         <v>43453</v>
@@ -16753,7 +16753,7 @@
     </row>
     <row r="431" spans="1:12">
       <c r="A431" s="1">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B431" s="2">
         <v>43454</v>
@@ -16791,7 +16791,7 @@
     </row>
     <row r="432" spans="1:12">
       <c r="A432" s="1">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B432" s="2">
         <v>43455</v>
@@ -16829,7 +16829,7 @@
     </row>
     <row r="433" spans="1:12">
       <c r="A433" s="1">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B433" s="2">
         <v>43456</v>
@@ -16867,7 +16867,7 @@
     </row>
     <row r="434" spans="1:12">
       <c r="A434" s="1">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B434" s="2">
         <v>43457</v>
@@ -16905,7 +16905,7 @@
     </row>
     <row r="435" spans="1:12">
       <c r="A435" s="1">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B435" s="2">
         <v>43458</v>
@@ -16943,7 +16943,7 @@
     </row>
     <row r="436" spans="1:12">
       <c r="A436" s="1">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B436" s="2">
         <v>43459</v>
@@ -16981,7 +16981,7 @@
     </row>
     <row r="437" spans="1:12">
       <c r="A437" s="1">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B437" s="2">
         <v>43460</v>
@@ -17019,7 +17019,7 @@
     </row>
     <row r="438" spans="1:12">
       <c r="A438" s="1">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B438" s="2">
         <v>43461</v>
@@ -17057,7 +17057,7 @@
     </row>
     <row r="439" spans="1:12">
       <c r="A439" s="1">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B439" s="2">
         <v>43462</v>
@@ -17095,7 +17095,7 @@
     </row>
     <row r="440" spans="1:12">
       <c r="A440" s="1">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B440" s="2">
         <v>43463</v>
@@ -17133,7 +17133,7 @@
     </row>
     <row r="441" spans="1:12">
       <c r="A441" s="1">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B441" s="2">
         <v>43464</v>
@@ -17171,7 +17171,7 @@
     </row>
     <row r="442" spans="1:12">
       <c r="A442" s="1">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B442" s="2">
         <v>43465</v>
@@ -17209,7 +17209,7 @@
     </row>
     <row r="443" spans="1:12">
       <c r="A443" s="1">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B443" s="2">
         <v>43466</v>
@@ -17247,7 +17247,7 @@
     </row>
     <row r="444" spans="1:12">
       <c r="A444" s="1">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B444" s="2">
         <v>43467</v>
@@ -17285,7 +17285,7 @@
     </row>
     <row r="445" spans="1:12">
       <c r="A445" s="1">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B445" s="2">
         <v>43468</v>
@@ -17323,7 +17323,7 @@
     </row>
     <row r="446" spans="1:12">
       <c r="A446" s="1">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B446" s="2">
         <v>43469</v>
@@ -17361,7 +17361,7 @@
     </row>
     <row r="447" spans="1:12">
       <c r="A447" s="1">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B447" s="2">
         <v>43470</v>
@@ -17399,7 +17399,7 @@
     </row>
     <row r="448" spans="1:12">
       <c r="A448" s="1">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B448" s="2">
         <v>43471</v>
@@ -17437,7 +17437,7 @@
     </row>
     <row r="449" spans="1:12">
       <c r="A449" s="1">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B449" s="2">
         <v>43472</v>
@@ -17475,7 +17475,7 @@
     </row>
     <row r="450" spans="1:12">
       <c r="A450" s="1">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B450" s="2">
         <v>43473</v>
@@ -17513,7 +17513,7 @@
     </row>
     <row r="451" spans="1:12">
       <c r="A451" s="1">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B451" s="2">
         <v>43474</v>
@@ -17551,7 +17551,7 @@
     </row>
     <row r="452" spans="1:12">
       <c r="A452" s="1">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B452" s="2">
         <v>43475</v>
@@ -17589,7 +17589,7 @@
     </row>
     <row r="453" spans="1:12">
       <c r="A453" s="1">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B453" s="2">
         <v>43476</v>
@@ -17627,7 +17627,7 @@
     </row>
     <row r="454" spans="1:12">
       <c r="A454" s="1">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B454" s="2">
         <v>43477</v>
@@ -17665,7 +17665,7 @@
     </row>
     <row r="455" spans="1:12">
       <c r="A455" s="1">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B455" s="2">
         <v>43478</v>
@@ -17703,7 +17703,7 @@
     </row>
     <row r="456" spans="1:12">
       <c r="A456" s="1">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B456" s="2">
         <v>43479</v>
@@ -17741,7 +17741,7 @@
     </row>
     <row r="457" spans="1:12">
       <c r="A457" s="1">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B457" s="2">
         <v>43480</v>
@@ -17779,7 +17779,7 @@
     </row>
     <row r="458" spans="1:12">
       <c r="A458" s="1">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B458" s="2">
         <v>43481</v>
@@ -17817,7 +17817,7 @@
     </row>
     <row r="459" spans="1:12">
       <c r="A459" s="1">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B459" s="2">
         <v>43482</v>
@@ -17855,7 +17855,7 @@
     </row>
     <row r="460" spans="1:12">
       <c r="A460" s="1">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B460" s="2">
         <v>43483</v>
@@ -17893,7 +17893,7 @@
     </row>
     <row r="461" spans="1:12">
       <c r="A461" s="1">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B461" s="2">
         <v>43484</v>
@@ -17931,7 +17931,7 @@
     </row>
     <row r="462" spans="1:12">
       <c r="A462" s="1">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B462" s="2">
         <v>43485</v>
@@ -17969,7 +17969,7 @@
     </row>
     <row r="463" spans="1:12">
       <c r="A463" s="1">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B463" s="2">
         <v>43486</v>
@@ -18007,7 +18007,7 @@
     </row>
     <row r="464" spans="1:12">
       <c r="A464" s="1">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B464" s="2">
         <v>43487</v>
@@ -18045,7 +18045,7 @@
     </row>
     <row r="465" spans="1:12">
       <c r="A465" s="1">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B465" s="2">
         <v>43488</v>
@@ -18083,7 +18083,7 @@
     </row>
     <row r="466" spans="1:12">
       <c r="A466" s="1">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B466" s="2">
         <v>43489</v>
@@ -18121,7 +18121,7 @@
     </row>
     <row r="467" spans="1:12">
       <c r="A467" s="1">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B467" s="2">
         <v>43490</v>
@@ -18159,7 +18159,7 @@
     </row>
     <row r="468" spans="1:12">
       <c r="A468" s="1">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B468" s="2">
         <v>43491</v>
@@ -18197,7 +18197,7 @@
     </row>
     <row r="469" spans="1:12">
       <c r="A469" s="1">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B469" s="2">
         <v>43492</v>
@@ -18235,7 +18235,7 @@
     </row>
     <row r="470" spans="1:12">
       <c r="A470" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B470" s="2">
         <v>43493</v>
@@ -18273,7 +18273,7 @@
     </row>
     <row r="471" spans="1:12">
       <c r="A471" s="1">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B471" s="2">
         <v>43494</v>
@@ -18311,7 +18311,7 @@
     </row>
     <row r="472" spans="1:12">
       <c r="A472" s="1">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B472" s="2">
         <v>43495</v>
@@ -18349,7 +18349,7 @@
     </row>
     <row r="473" spans="1:12">
       <c r="A473" s="1">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B473" s="2">
         <v>43496</v>
@@ -18387,7 +18387,7 @@
     </row>
     <row r="474" spans="1:12">
       <c r="A474" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B474" s="2">
         <v>43497</v>
@@ -18425,7 +18425,7 @@
     </row>
     <row r="475" spans="1:12">
       <c r="A475" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B475" s="2">
         <v>43498</v>
@@ -18463,7 +18463,7 @@
     </row>
     <row r="476" spans="1:12">
       <c r="A476" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B476" s="2">
         <v>43499</v>
@@ -18501,7 +18501,7 @@
     </row>
     <row r="477" spans="1:12">
       <c r="A477" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B477" s="2">
         <v>43500</v>
@@ -18539,7 +18539,7 @@
     </row>
     <row r="478" spans="1:12">
       <c r="A478" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B478" s="2">
         <v>43501</v>
@@ -18577,7 +18577,7 @@
     </row>
     <row r="479" spans="1:12">
       <c r="A479" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B479" s="2">
         <v>43502</v>
@@ -18615,7 +18615,7 @@
     </row>
     <row r="480" spans="1:12">
       <c r="A480" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B480" s="2">
         <v>43503</v>
@@ -18653,7 +18653,7 @@
     </row>
     <row r="481" spans="1:12">
       <c r="A481" s="1">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B481" s="2">
         <v>43504</v>
@@ -18691,7 +18691,7 @@
     </row>
     <row r="482" spans="1:12">
       <c r="A482" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B482" s="2">
         <v>43505</v>
@@ -18729,7 +18729,7 @@
     </row>
     <row r="483" spans="1:12">
       <c r="A483" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B483" s="2">
         <v>43506</v>
@@ -18767,7 +18767,7 @@
     </row>
     <row r="484" spans="1:12">
       <c r="A484" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B484" s="2">
         <v>43507</v>
@@ -18805,7 +18805,7 @@
     </row>
     <row r="485" spans="1:12">
       <c r="A485" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B485" s="2">
         <v>43508</v>
@@ -18843,7 +18843,7 @@
     </row>
     <row r="486" spans="1:12">
       <c r="A486" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B486" s="2">
         <v>43509</v>
@@ -18881,7 +18881,7 @@
     </row>
     <row r="487" spans="1:12">
       <c r="A487" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B487" s="2">
         <v>43510</v>
@@ -18919,7 +18919,7 @@
     </row>
     <row r="488" spans="1:12">
       <c r="A488" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B488" s="2">
         <v>43511</v>
@@ -18957,7 +18957,7 @@
     </row>
     <row r="489" spans="1:12">
       <c r="A489" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B489" s="2">
         <v>43512</v>
@@ -18995,7 +18995,7 @@
     </row>
     <row r="490" spans="1:12">
       <c r="A490" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B490" s="2">
         <v>43513</v>
@@ -19033,7 +19033,7 @@
     </row>
     <row r="491" spans="1:12">
       <c r="A491" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B491" s="2">
         <v>43514</v>
@@ -19071,7 +19071,7 @@
     </row>
     <row r="492" spans="1:12">
       <c r="A492" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B492" s="2">
         <v>43515</v>
@@ -19109,7 +19109,7 @@
     </row>
     <row r="493" spans="1:12">
       <c r="A493" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B493" s="2">
         <v>43516</v>
@@ -19147,7 +19147,7 @@
     </row>
     <row r="494" spans="1:12">
       <c r="A494" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B494" s="2">
         <v>43517</v>
@@ -19185,7 +19185,7 @@
     </row>
     <row r="495" spans="1:12">
       <c r="A495" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B495" s="2">
         <v>43518</v>
@@ -19223,7 +19223,7 @@
     </row>
     <row r="496" spans="1:12">
       <c r="A496" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B496" s="2">
         <v>43519</v>
@@ -19261,7 +19261,7 @@
     </row>
     <row r="497" spans="1:12">
       <c r="A497" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B497" s="2">
         <v>43520</v>
@@ -19299,7 +19299,7 @@
     </row>
     <row r="498" spans="1:12">
       <c r="A498" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B498" s="2">
         <v>43521</v>
@@ -19337,7 +19337,7 @@
     </row>
     <row r="499" spans="1:12">
       <c r="A499" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B499" s="2">
         <v>43522</v>
@@ -19375,7 +19375,7 @@
     </row>
     <row r="500" spans="1:12">
       <c r="A500" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B500" s="2">
         <v>43523</v>
@@ -19413,7 +19413,7 @@
     </row>
     <row r="501" spans="1:12">
       <c r="A501" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B501" s="2">
         <v>43524</v>
@@ -19451,7 +19451,7 @@
     </row>
     <row r="502" spans="1:12">
       <c r="A502" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B502" s="2">
         <v>43525</v>
@@ -19489,7 +19489,7 @@
     </row>
     <row r="503" spans="1:12">
       <c r="A503" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B503" s="2">
         <v>43526</v>
@@ -19527,7 +19527,7 @@
     </row>
     <row r="504" spans="1:12">
       <c r="A504" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B504" s="2">
         <v>43527</v>
@@ -19561,6 +19561,44 @@
       </c>
       <c r="L504">
         <v>5.922899510092486</v>
+      </c>
+    </row>
+    <row r="505" spans="1:12">
+      <c r="A505" s="1">
+        <v>0</v>
+      </c>
+      <c r="B505" s="2">
+        <v>43528</v>
+      </c>
+      <c r="C505">
+        <v>3845.09</v>
+      </c>
+      <c r="D505">
+        <v>3867.38</v>
+      </c>
+      <c r="E505">
+        <v>3733.75</v>
+      </c>
+      <c r="F505">
+        <v>3761.56</v>
+      </c>
+      <c r="G505">
+        <v>9029175788</v>
+      </c>
+      <c r="H505">
+        <v>66094551587</v>
+      </c>
+      <c r="I505">
+        <v>-0.02250664740755148</v>
+      </c>
+      <c r="J505">
+        <v>0.02634605937350771</v>
+      </c>
+      <c r="K505">
+        <v>0.009049695223880027</v>
+      </c>
+      <c r="L505">
+        <v>5.414498483212308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>